<commit_message>
NC-2.3 - Tela de cadastro
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\AppNotificacoesCrimesCidade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F25EC68-5F5E-4556-8EDF-46983824A228}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68E06BA5-0399-47A6-8625-F5DCB3AE3DF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="780" windowWidth="19440" windowHeight="10440" xr2:uid="{996D4097-5510-4348-97EC-A204A307EBA8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{996D4097-5510-4348-97EC-A204A307EBA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="101">
   <si>
     <t>Descrição</t>
   </si>
@@ -339,9 +339,6 @@
   </si>
   <si>
     <t>1.10</t>
-  </si>
-  <si>
-    <t>Fazendo</t>
   </si>
   <si>
     <t>A definir</t>
@@ -366,7 +363,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -376,12 +373,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -404,7 +395,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -429,10 +420,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -769,8 +756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94151779-DED3-44C5-B19B-FEA501E890E9}">
   <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -844,14 +831,14 @@
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
       <c r="B5" s="8"/>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="11" t="s">
-        <v>101</v>
+      <c r="E5" s="7" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -883,40 +870,40 @@
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>
       <c r="B8" s="8"/>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="11" t="s">
-        <v>101</v>
+      <c r="E8" s="7" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="9"/>
       <c r="B9" s="8"/>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="11" t="s">
-        <v>101</v>
+      <c r="E9" s="7" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
       <c r="B10" s="8"/>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="11" t="s">
-        <v>101</v>
+      <c r="E10" s="7" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -939,14 +926,14 @@
       <c r="B12" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="7" t="s">
-        <v>100</v>
+      <c r="E12" s="5" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -962,11 +949,14 @@
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
       <c r="B14" s="8"/>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="4" t="s">
         <v>33</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
NC-3.1 - Tela home + integração api maps google + integração api places google
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\AppNotificacoesCrimesCidade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68E06BA5-0399-47A6-8625-F5DCB3AE3DF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{389C8AE9-B5D1-41F0-963F-F5CEB6AD6F0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{996D4097-5510-4348-97EC-A204A307EBA8}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="104">
   <si>
     <t>Descrição</t>
   </si>
@@ -342,6 +342,15 @@
   </si>
   <si>
     <t>A definir</t>
+  </si>
+  <si>
+    <t>Fazendo</t>
+  </si>
+  <si>
+    <t>Mover projeto front end para repositório da organização</t>
+  </si>
+  <si>
+    <t>1.11</t>
   </si>
 </sst>
 </file>
@@ -363,7 +372,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -382,6 +391,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -395,7 +410,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -415,10 +430,20 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -754,10 +779,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94151779-DED3-44C5-B19B-FEA501E890E9}">
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -786,10 +811,10 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9">
+      <c r="A2" s="12">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="11" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -803,8 +828,8 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
-      <c r="B3" s="8"/>
+      <c r="A3" s="12"/>
+      <c r="B3" s="11"/>
       <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
@@ -816,8 +841,8 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
-      <c r="B4" s="8"/>
+      <c r="A4" s="12"/>
+      <c r="B4" s="11"/>
       <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
@@ -829,8 +854,8 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" s="8"/>
+      <c r="A5" s="12"/>
+      <c r="B5" s="11"/>
       <c r="C5" s="6" t="s">
         <v>8</v>
       </c>
@@ -842,8 +867,8 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
-      <c r="B6" s="8"/>
+      <c r="A6" s="12"/>
+      <c r="B6" s="11"/>
       <c r="C6" s="4" t="s">
         <v>9</v>
       </c>
@@ -855,8 +880,8 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="8"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="11"/>
       <c r="C7" s="4" t="s">
         <v>10</v>
       </c>
@@ -868,8 +893,8 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="B8" s="8"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="11"/>
       <c r="C8" s="6" t="s">
         <v>11</v>
       </c>
@@ -881,8 +906,8 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="8"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="11"/>
       <c r="C9" s="6" t="s">
         <v>12</v>
       </c>
@@ -894,8 +919,8 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="8"/>
+      <c r="A10" s="12"/>
+      <c r="B10" s="11"/>
       <c r="C10" s="6" t="s">
         <v>13</v>
       </c>
@@ -907,8 +932,8 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
-      <c r="B11" s="8"/>
+      <c r="A11" s="12"/>
+      <c r="B11" s="11"/>
       <c r="C11" s="4" t="s">
         <v>98</v>
       </c>
@@ -919,396 +944,412 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="9">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="12">
         <v>2</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B13" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C13" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D13" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E13" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="1" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="12"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="4" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="12"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D15" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E15" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="1" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="12"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="1" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="12"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="9">
+    <row r="18" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="12">
         <v>3</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B18" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C18" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D18" s="9" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="1" t="s">
+      <c r="E18" s="10" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="12"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="9"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="1" t="s">
+    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="12"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="9"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="1" t="s">
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="12"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="9">
+    <row r="22" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="12">
         <v>4</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B22" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="9"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="1" t="s">
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="12"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="9"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="1" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="12"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D24" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="9"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="1" t="s">
+    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="12"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="9"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="1" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="12"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="9"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="1" t="s">
+    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="12"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="9">
+    <row r="28" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="12">
         <v>5</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B28" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="9"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="1" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="12"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D29" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="9"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="1" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="12"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D30" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="9"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="1" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="12"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D31" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="9">
+    <row r="32" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="12">
         <v>6</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B32" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D32" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="9"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="1" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="12"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D33" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="9"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="1" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="12"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D34" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="9"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="1" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="12"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A35" s="9">
+    <row r="36" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A36" s="12">
         <v>7</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B36" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C36" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D36" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="9"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="1" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="12"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D37" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A37" s="9"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="1" t="s">
+    <row r="38" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A38" s="12"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D38" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="9"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="1" t="s">
+    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="12"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D39" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A39" s="9">
+    <row r="40" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" s="12">
         <v>8</v>
       </c>
-      <c r="B39" s="8" t="s">
+      <c r="B40" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C40" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D40" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="9"/>
-      <c r="B40" s="8"/>
-      <c r="C40" s="1" t="s">
+    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="12"/>
+      <c r="B41" s="11"/>
+      <c r="C41" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="D41" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A41" s="2">
+    <row r="42" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
         <v>9</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B42" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C42" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="D42" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A42" s="9">
+    <row r="43" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A43" s="12">
         <v>10</v>
       </c>
-      <c r="B42" s="8" t="s">
+      <c r="B43" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C43" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D43" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="9"/>
-      <c r="B43" s="8"/>
-      <c r="C43" s="1" t="s">
+    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="12"/>
+      <c r="B44" s="11"/>
+      <c r="C44" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D44" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="9"/>
-      <c r="B44" s="8"/>
-    </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="9"/>
-      <c r="B45" s="8"/>
+      <c r="A45" s="12"/>
+      <c r="B45" s="11"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="12"/>
+      <c r="B46" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B2:B11"/>
     <mergeCell ref="A2:A11"/>
-    <mergeCell ref="B12:B16"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="B17:B20"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="B21:B26"/>
-    <mergeCell ref="A21:A26"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="B31:B34"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="B42:B45"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="B35:B38"/>
-    <mergeCell ref="A35:A38"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B13:B17"/>
+    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="B2:B12"/>
+    <mergeCell ref="B22:B27"/>
+    <mergeCell ref="A22:A27"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="B32:B35"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="B43:B46"/>
+    <mergeCell ref="A43:A46"/>
+    <mergeCell ref="B36:B39"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="A40:A41"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
NC-4.1 4.3 4.5 - Desenvolvimento das telas de cadastro de ocorrências
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\AppNotificacoesCrimesCidade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{389C8AE9-B5D1-41F0-963F-F5CEB6AD6F0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D77A0C85-E869-49C5-AD43-339207CCBDBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{996D4097-5510-4348-97EC-A204A307EBA8}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="106">
   <si>
     <t>Descrição</t>
   </si>
@@ -351,6 +351,12 @@
   </si>
   <si>
     <t>1.11</t>
+  </si>
+  <si>
+    <t>3.5</t>
+  </si>
+  <si>
+    <t>Passar para o backend a rotina de pesquisa de endereço</t>
   </si>
 </sst>
 </file>
@@ -410,7 +416,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -436,14 +442,18 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -779,10 +789,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94151779-DED3-44C5-B19B-FEA501E890E9}">
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -811,10 +821,10 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12">
+      <c r="A2" s="14">
         <v>1</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="15" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -828,8 +838,8 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
-      <c r="B3" s="11"/>
+      <c r="A3" s="14"/>
+      <c r="B3" s="15"/>
       <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
@@ -841,8 +851,8 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="11"/>
+      <c r="A4" s="14"/>
+      <c r="B4" s="15"/>
       <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
@@ -854,8 +864,8 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
-      <c r="B5" s="11"/>
+      <c r="A5" s="14"/>
+      <c r="B5" s="15"/>
       <c r="C5" s="6" t="s">
         <v>8</v>
       </c>
@@ -867,8 +877,8 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
-      <c r="B6" s="11"/>
+      <c r="A6" s="14"/>
+      <c r="B6" s="15"/>
       <c r="C6" s="4" t="s">
         <v>9</v>
       </c>
@@ -880,8 +890,8 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
-      <c r="B7" s="11"/>
+      <c r="A7" s="14"/>
+      <c r="B7" s="15"/>
       <c r="C7" s="4" t="s">
         <v>10</v>
       </c>
@@ -893,8 +903,8 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
-      <c r="B8" s="11"/>
+      <c r="A8" s="14"/>
+      <c r="B8" s="15"/>
       <c r="C8" s="6" t="s">
         <v>11</v>
       </c>
@@ -906,8 +916,8 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
-      <c r="B9" s="11"/>
+      <c r="A9" s="14"/>
+      <c r="B9" s="15"/>
       <c r="C9" s="6" t="s">
         <v>12</v>
       </c>
@@ -919,8 +929,8 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
-      <c r="B10" s="11"/>
+      <c r="A10" s="14"/>
+      <c r="B10" s="15"/>
       <c r="C10" s="6" t="s">
         <v>13</v>
       </c>
@@ -932,8 +942,8 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
-      <c r="B11" s="11"/>
+      <c r="A11" s="14"/>
+      <c r="B11" s="15"/>
       <c r="C11" s="4" t="s">
         <v>98</v>
       </c>
@@ -946,22 +956,22 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="13" t="s">
+      <c r="B12" s="15"/>
+      <c r="C12" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="E12" s="11" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="12">
+      <c r="A13" s="14">
         <v>2</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="15" t="s">
         <v>25</v>
       </c>
       <c r="C13" s="4" t="s">
@@ -975,8 +985,8 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
-      <c r="B14" s="11"/>
+      <c r="A14" s="14"/>
+      <c r="B14" s="15"/>
       <c r="C14" s="1" t="s">
         <v>27</v>
       </c>
@@ -985,8 +995,8 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
-      <c r="B15" s="11"/>
+      <c r="A15" s="14"/>
+      <c r="B15" s="15"/>
       <c r="C15" s="4" t="s">
         <v>28</v>
       </c>
@@ -998,8 +1008,8 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
-      <c r="B16" s="11"/>
+      <c r="A16" s="14"/>
+      <c r="B16" s="15"/>
       <c r="C16" s="1" t="s">
         <v>29</v>
       </c>
@@ -1008,8 +1018,8 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
-      <c r="B17" s="11"/>
+      <c r="A17" s="14"/>
+      <c r="B17" s="15"/>
       <c r="C17" s="1" t="s">
         <v>30</v>
       </c>
@@ -1018,25 +1028,25 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="12">
+      <c r="A18" s="14">
         <v>3</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="E18" s="10" t="s">
-        <v>101</v>
+      <c r="E18" s="5" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
-      <c r="B19" s="11"/>
+      <c r="A19" s="14"/>
+      <c r="B19" s="15"/>
       <c r="C19" s="1" t="s">
         <v>38</v>
       </c>
@@ -1045,8 +1055,8 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="12"/>
-      <c r="B20" s="11"/>
+      <c r="A20" s="14"/>
+      <c r="B20" s="15"/>
       <c r="C20" s="1" t="s">
         <v>39</v>
       </c>
@@ -1055,301 +1065,318 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="12"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="1" t="s">
+      <c r="A21" s="14"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="12">
+      <c r="E21" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="14"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="E22" s="13"/>
+    </row>
+    <row r="23" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="14">
         <v>4</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B23" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C23" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D23" s="9" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="1" t="s">
+      <c r="E23" s="10" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="14"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D24" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="12"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="1" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="14"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="12"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="1" t="s">
+    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="14"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="12"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="1" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="14"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="12"/>
-      <c r="B27" s="11"/>
-      <c r="C27" s="1" t="s">
+    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="14"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="12">
+    <row r="29" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="14">
         <v>5</v>
       </c>
-      <c r="B28" s="11" t="s">
+      <c r="B29" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D29" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="12"/>
-      <c r="B29" s="11"/>
-      <c r="C29" s="1" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="14"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D30" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="12"/>
-      <c r="B30" s="11"/>
-      <c r="C30" s="1" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="14"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D31" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="12"/>
-      <c r="B31" s="11"/>
-      <c r="C31" s="1" t="s">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="14"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D32" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="12">
+    <row r="33" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="14">
         <v>6</v>
       </c>
-      <c r="B32" s="11" t="s">
+      <c r="B33" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D33" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="12"/>
-      <c r="B33" s="11"/>
-      <c r="C33" s="1" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="14"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D34" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="12"/>
-      <c r="B34" s="11"/>
-      <c r="C34" s="1" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="14"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="12"/>
-      <c r="B35" s="11"/>
-      <c r="C35" s="1" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="14"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D36" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A36" s="12">
+    <row r="37" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A37" s="14">
         <v>7</v>
       </c>
-      <c r="B36" s="11" t="s">
+      <c r="B37" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C37" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D37" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="12"/>
-      <c r="B37" s="11"/>
-      <c r="C37" s="1" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="14"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D38" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A38" s="12"/>
-      <c r="B38" s="11"/>
-      <c r="C38" s="1" t="s">
+    <row r="39" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A39" s="14"/>
+      <c r="B39" s="15"/>
+      <c r="C39" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D39" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="12"/>
-      <c r="B39" s="11"/>
-      <c r="C39" s="1" t="s">
+    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="14"/>
+      <c r="B40" s="15"/>
+      <c r="C40" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D40" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A40" s="12">
+    <row r="41" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A41" s="14">
         <v>8</v>
       </c>
-      <c r="B40" s="11" t="s">
+      <c r="B41" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C41" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="D41" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="12"/>
-      <c r="B41" s="11"/>
-      <c r="C41" s="1" t="s">
+    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="14"/>
+      <c r="B42" s="15"/>
+      <c r="C42" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="D42" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A42" s="2">
+    <row r="43" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
         <v>9</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B43" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C43" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D43" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A43" s="12">
+    <row r="44" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A44" s="14">
         <v>10</v>
       </c>
-      <c r="B43" s="11" t="s">
+      <c r="B44" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C44" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D44" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="12"/>
-      <c r="B44" s="11"/>
-      <c r="C44" s="1" t="s">
+    <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="14"/>
+      <c r="B45" s="15"/>
+      <c r="C45" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="D45" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="12"/>
-      <c r="B45" s="11"/>
-    </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="12"/>
-      <c r="B46" s="11"/>
+      <c r="A46" s="14"/>
+      <c r="B46" s="15"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="14"/>
+      <c r="B47" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B44:B47"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="B37:B40"/>
+    <mergeCell ref="A37:A40"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B23:B28"/>
+    <mergeCell ref="A23:A28"/>
+    <mergeCell ref="B29:B32"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="B33:B36"/>
+    <mergeCell ref="A33:A36"/>
     <mergeCell ref="A2:A11"/>
     <mergeCell ref="B13:B17"/>
     <mergeCell ref="A13:A17"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="A18:A21"/>
     <mergeCell ref="B2:B12"/>
-    <mergeCell ref="B22:B27"/>
-    <mergeCell ref="A22:A27"/>
-    <mergeCell ref="B28:B31"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="B32:B35"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="B43:B46"/>
-    <mergeCell ref="A43:A46"/>
-    <mergeCell ref="B36:B39"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="A18:A22"/>
+    <mergeCell ref="B18:B22"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
NC-1.4 - Criação do projeto de backend
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\AppNotificacoesCrimesCidade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D77A0C85-E869-49C5-AD43-339207CCBDBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3572287A-D4CF-4940-A532-C8817213FA4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{996D4097-5510-4348-97EC-A204A307EBA8}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="106">
   <si>
     <t>Descrição</t>
   </si>
@@ -450,10 +450,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -791,8 +791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94151779-DED3-44C5-B19B-FEA501E890E9}">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -821,10 +821,10 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14">
+      <c r="A2" s="15">
         <v>1</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="14" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -838,8 +838,8 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="15"/>
+      <c r="A3" s="15"/>
+      <c r="B3" s="14"/>
       <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
@@ -851,8 +851,8 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="15"/>
+      <c r="A4" s="15"/>
+      <c r="B4" s="14"/>
       <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
@@ -864,21 +864,21 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="6" t="s">
+      <c r="A5" s="15"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="10" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="15"/>
+      <c r="A6" s="15"/>
+      <c r="B6" s="14"/>
       <c r="C6" s="4" t="s">
         <v>9</v>
       </c>
@@ -890,8 +890,8 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="15"/>
+      <c r="A7" s="15"/>
+      <c r="B7" s="14"/>
       <c r="C7" s="4" t="s">
         <v>10</v>
       </c>
@@ -903,8 +903,8 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
-      <c r="B8" s="15"/>
+      <c r="A8" s="15"/>
+      <c r="B8" s="14"/>
       <c r="C8" s="6" t="s">
         <v>11</v>
       </c>
@@ -916,8 +916,8 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="15"/>
+      <c r="A9" s="15"/>
+      <c r="B9" s="14"/>
       <c r="C9" s="6" t="s">
         <v>12</v>
       </c>
@@ -929,8 +929,8 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
-      <c r="B10" s="15"/>
+      <c r="A10" s="15"/>
+      <c r="B10" s="14"/>
       <c r="C10" s="6" t="s">
         <v>13</v>
       </c>
@@ -942,8 +942,8 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="15"/>
+      <c r="A11" s="15"/>
+      <c r="B11" s="14"/>
       <c r="C11" s="4" t="s">
         <v>98</v>
       </c>
@@ -956,7 +956,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
-      <c r="B12" s="15"/>
+      <c r="B12" s="14"/>
       <c r="C12" s="11" t="s">
         <v>102</v>
       </c>
@@ -968,10 +968,10 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14">
+      <c r="A13" s="15">
         <v>2</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="14" t="s">
         <v>25</v>
       </c>
       <c r="C13" s="4" t="s">
@@ -985,8 +985,8 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
-      <c r="B14" s="15"/>
+      <c r="A14" s="15"/>
+      <c r="B14" s="14"/>
       <c r="C14" s="1" t="s">
         <v>27</v>
       </c>
@@ -995,8 +995,8 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
-      <c r="B15" s="15"/>
+      <c r="A15" s="15"/>
+      <c r="B15" s="14"/>
       <c r="C15" s="4" t="s">
         <v>28</v>
       </c>
@@ -1008,8 +1008,8 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
-      <c r="B16" s="15"/>
+      <c r="A16" s="15"/>
+      <c r="B16" s="14"/>
       <c r="C16" s="1" t="s">
         <v>29</v>
       </c>
@@ -1018,8 +1018,8 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
-      <c r="B17" s="15"/>
+      <c r="A17" s="15"/>
+      <c r="B17" s="14"/>
       <c r="C17" s="1" t="s">
         <v>30</v>
       </c>
@@ -1028,10 +1028,10 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="14">
+      <c r="A18" s="15">
         <v>3</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="14" t="s">
         <v>36</v>
       </c>
       <c r="C18" s="4" t="s">
@@ -1045,8 +1045,8 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
-      <c r="B19" s="15"/>
+      <c r="A19" s="15"/>
+      <c r="B19" s="14"/>
       <c r="C19" s="1" t="s">
         <v>38</v>
       </c>
@@ -1055,8 +1055,8 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
-      <c r="B20" s="15"/>
+      <c r="A20" s="15"/>
+      <c r="B20" s="14"/>
       <c r="C20" s="1" t="s">
         <v>39</v>
       </c>
@@ -1065,8 +1065,8 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
-      <c r="B21" s="15"/>
+      <c r="A21" s="15"/>
+      <c r="B21" s="14"/>
       <c r="C21" s="4" t="s">
         <v>40</v>
       </c>
@@ -1078,8 +1078,8 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="14"/>
-      <c r="B22" s="15"/>
+      <c r="A22" s="15"/>
+      <c r="B22" s="14"/>
       <c r="C22" s="12" t="s">
         <v>105</v>
       </c>
@@ -1089,25 +1089,25 @@
       <c r="E22" s="13"/>
     </row>
     <row r="23" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="14">
+      <c r="A23" s="15">
         <v>4</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="D23" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E23" s="10" t="s">
-        <v>101</v>
+      <c r="E23" s="5" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="14"/>
-      <c r="B24" s="15"/>
+      <c r="A24" s="15"/>
+      <c r="B24" s="14"/>
       <c r="C24" s="1" t="s">
         <v>47</v>
       </c>
@@ -1116,18 +1116,21 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="14"/>
-      <c r="B25" s="15"/>
-      <c r="C25" s="1" t="s">
+      <c r="A25" s="15"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" s="4" t="s">
         <v>54</v>
       </c>
+      <c r="E25" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="14"/>
-      <c r="B26" s="15"/>
+      <c r="A26" s="15"/>
+      <c r="B26" s="14"/>
       <c r="C26" s="1" t="s">
         <v>49</v>
       </c>
@@ -1136,18 +1139,21 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="14"/>
-      <c r="B27" s="15"/>
-      <c r="C27" s="1" t="s">
+      <c r="A27" s="15"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D27" s="4" t="s">
         <v>56</v>
       </c>
+      <c r="E27" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="14"/>
-      <c r="B28" s="15"/>
+      <c r="A28" s="15"/>
+      <c r="B28" s="14"/>
       <c r="C28" s="1" t="s">
         <v>51</v>
       </c>
@@ -1156,10 +1162,10 @@
       </c>
     </row>
     <row r="29" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="14">
+      <c r="A29" s="15">
         <v>5</v>
       </c>
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="14" t="s">
         <v>58</v>
       </c>
       <c r="C29" s="1" t="s">
@@ -1170,8 +1176,8 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="14"/>
-      <c r="B30" s="15"/>
+      <c r="A30" s="15"/>
+      <c r="B30" s="14"/>
       <c r="C30" s="1" t="s">
         <v>60</v>
       </c>
@@ -1180,8 +1186,8 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="14"/>
-      <c r="B31" s="15"/>
+      <c r="A31" s="15"/>
+      <c r="B31" s="14"/>
       <c r="C31" s="1" t="s">
         <v>61</v>
       </c>
@@ -1190,8 +1196,8 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="14"/>
-      <c r="B32" s="15"/>
+      <c r="A32" s="15"/>
+      <c r="B32" s="14"/>
       <c r="C32" s="1" t="s">
         <v>62</v>
       </c>
@@ -1200,10 +1206,10 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="14">
+      <c r="A33" s="15">
         <v>6</v>
       </c>
-      <c r="B33" s="15" t="s">
+      <c r="B33" s="14" t="s">
         <v>67</v>
       </c>
       <c r="C33" s="1" t="s">
@@ -1214,8 +1220,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="14"/>
-      <c r="B34" s="15"/>
+      <c r="A34" s="15"/>
+      <c r="B34" s="14"/>
       <c r="C34" s="1" t="s">
         <v>69</v>
       </c>
@@ -1224,8 +1230,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="14"/>
-      <c r="B35" s="15"/>
+      <c r="A35" s="15"/>
+      <c r="B35" s="14"/>
       <c r="C35" s="1" t="s">
         <v>70</v>
       </c>
@@ -1234,8 +1240,8 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="14"/>
-      <c r="B36" s="15"/>
+      <c r="A36" s="15"/>
+      <c r="B36" s="14"/>
       <c r="C36" s="1" t="s">
         <v>71</v>
       </c>
@@ -1244,10 +1250,10 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A37" s="14">
+      <c r="A37" s="15">
         <v>7</v>
       </c>
-      <c r="B37" s="15" t="s">
+      <c r="B37" s="14" t="s">
         <v>76</v>
       </c>
       <c r="C37" s="1" t="s">
@@ -1258,8 +1264,8 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="14"/>
-      <c r="B38" s="15"/>
+      <c r="A38" s="15"/>
+      <c r="B38" s="14"/>
       <c r="C38" s="1" t="s">
         <v>77</v>
       </c>
@@ -1268,8 +1274,8 @@
       </c>
     </row>
     <row r="39" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A39" s="14"/>
-      <c r="B39" s="15"/>
+      <c r="A39" s="15"/>
+      <c r="B39" s="14"/>
       <c r="C39" s="1" t="s">
         <v>79</v>
       </c>
@@ -1278,8 +1284,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="14"/>
-      <c r="B40" s="15"/>
+      <c r="A40" s="15"/>
+      <c r="B40" s="14"/>
       <c r="C40" s="1" t="s">
         <v>83</v>
       </c>
@@ -1288,10 +1294,10 @@
       </c>
     </row>
     <row r="41" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A41" s="14">
+      <c r="A41" s="15">
         <v>8</v>
       </c>
-      <c r="B41" s="15" t="s">
+      <c r="B41" s="14" t="s">
         <v>85</v>
       </c>
       <c r="C41" s="1" t="s">
@@ -1302,8 +1308,8 @@
       </c>
     </row>
     <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="14"/>
-      <c r="B42" s="15"/>
+      <c r="A42" s="15"/>
+      <c r="B42" s="14"/>
       <c r="C42" s="1" t="s">
         <v>87</v>
       </c>
@@ -1326,10 +1332,10 @@
       </c>
     </row>
     <row r="44" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A44" s="14">
+      <c r="A44" s="15">
         <v>10</v>
       </c>
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="14" t="s">
         <v>93</v>
       </c>
       <c r="C44" s="1" t="s">
@@ -1340,8 +1346,8 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="14"/>
-      <c r="B45" s="15"/>
+      <c r="A45" s="15"/>
+      <c r="B45" s="14"/>
       <c r="C45" s="1" t="s">
         <v>95</v>
       </c>
@@ -1350,33 +1356,33 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="14"/>
-      <c r="B46" s="15"/>
+      <c r="A46" s="15"/>
+      <c r="B46" s="14"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="14"/>
-      <c r="B47" s="15"/>
+      <c r="A47" s="15"/>
+      <c r="B47" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A2:A11"/>
+    <mergeCell ref="B13:B17"/>
+    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="B2:B12"/>
+    <mergeCell ref="A18:A22"/>
+    <mergeCell ref="B18:B22"/>
+    <mergeCell ref="B23:B28"/>
+    <mergeCell ref="A23:A28"/>
+    <mergeCell ref="B29:B32"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="B33:B36"/>
+    <mergeCell ref="A33:A36"/>
     <mergeCell ref="B44:B47"/>
     <mergeCell ref="A44:A47"/>
     <mergeCell ref="B37:B40"/>
     <mergeCell ref="A37:A40"/>
     <mergeCell ref="B41:B42"/>
     <mergeCell ref="A41:A42"/>
-    <mergeCell ref="B23:B28"/>
-    <mergeCell ref="A23:A28"/>
-    <mergeCell ref="B29:B32"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="B33:B36"/>
-    <mergeCell ref="A33:A36"/>
-    <mergeCell ref="A2:A11"/>
-    <mergeCell ref="B13:B17"/>
-    <mergeCell ref="A13:A17"/>
-    <mergeCell ref="B2:B12"/>
-    <mergeCell ref="A18:A22"/>
-    <mergeCell ref="B18:B22"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
NC-1.8 - Estrutura inicial para uso do flyWay para versionamento do banco de dados
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\AppNotificacoesCrimesCidade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3572287A-D4CF-4940-A532-C8817213FA4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{390FDE29-3C40-4ADE-A615-B21B70A2AB0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{996D4097-5510-4348-97EC-A204A307EBA8}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="104">
   <si>
     <t>Descrição</t>
   </si>
@@ -345,12 +345,6 @@
   </si>
   <si>
     <t>Fazendo</t>
-  </si>
-  <si>
-    <t>Mover projeto front end para repositório da organização</t>
-  </si>
-  <si>
-    <t>1.11</t>
   </si>
   <si>
     <t>3.5</t>
@@ -416,7 +410,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -435,16 +429,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -789,10 +777,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94151779-DED3-44C5-B19B-FEA501E890E9}">
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -821,10 +809,10 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15">
+      <c r="A2" s="13">
         <v>1</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="12" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -838,8 +826,8 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
-      <c r="B3" s="14"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="12"/>
       <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
@@ -851,8 +839,8 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
-      <c r="B4" s="14"/>
+      <c r="A4" s="13"/>
+      <c r="B4" s="12"/>
       <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
@@ -864,21 +852,21 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="9" t="s">
+      <c r="A5" s="13"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="10" t="s">
-        <v>100</v>
+      <c r="E5" s="5" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
-      <c r="B6" s="14"/>
+      <c r="A6" s="13"/>
+      <c r="B6" s="12"/>
       <c r="C6" s="4" t="s">
         <v>9</v>
       </c>
@@ -890,8 +878,8 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
-      <c r="B7" s="14"/>
+      <c r="A7" s="13"/>
+      <c r="B7" s="12"/>
       <c r="C7" s="4" t="s">
         <v>10</v>
       </c>
@@ -903,8 +891,8 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
-      <c r="B8" s="14"/>
+      <c r="A8" s="13"/>
+      <c r="B8" s="12"/>
       <c r="C8" s="6" t="s">
         <v>11</v>
       </c>
@@ -916,34 +904,34 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="15"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="6" t="s">
+      <c r="A9" s="13"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="7" t="s">
-        <v>100</v>
+      <c r="E9" s="5" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="6" t="s">
+      <c r="A10" s="13"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="7" t="s">
-        <v>100</v>
+      <c r="E10" s="9" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
-      <c r="B11" s="14"/>
+      <c r="A11" s="13"/>
+      <c r="B11" s="12"/>
       <c r="C11" s="4" t="s">
         <v>98</v>
       </c>
@@ -954,435 +942,422 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="11" t="s">
+    <row r="12" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="13">
+        <v>2</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="13"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="13"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="13"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="13"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="13">
+        <v>3</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="13"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="13"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="13"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="13"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="D21" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="D12" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="15">
-        <v>2</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="15"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="15"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="15"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="15">
-        <v>3</v>
-      </c>
-      <c r="B18" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="15"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="15"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="15"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="15"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="E22" s="13"/>
-    </row>
-    <row r="23" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="15">
+      <c r="E21" s="11"/>
+    </row>
+    <row r="22" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="13">
         <v>4</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B22" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C22" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D22" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E23" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="15"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="1" t="s">
+      <c r="E22" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="13"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="15"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="4" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="13"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D24" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E25" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="15"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="1" t="s">
+      <c r="E24" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="13"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="15"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="4" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="13"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D26" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E27" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="15"/>
-      <c r="B28" s="14"/>
+      <c r="E26" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="13"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="13">
+        <v>5</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>58</v>
+      </c>
       <c r="C28" s="1" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="15">
-        <v>5</v>
-      </c>
-      <c r="B29" s="14" t="s">
-        <v>58</v>
-      </c>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="13"/>
+      <c r="B29" s="12"/>
       <c r="C29" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="15"/>
-      <c r="B30" s="14"/>
+      <c r="A30" s="13"/>
+      <c r="B30" s="12"/>
       <c r="C30" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="15"/>
-      <c r="B31" s="14"/>
+      <c r="A31" s="13"/>
+      <c r="B31" s="12"/>
       <c r="C31" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="15"/>
-      <c r="B32" s="14"/>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="13">
+        <v>6</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="C32" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="15">
-        <v>6</v>
-      </c>
-      <c r="B33" s="14" t="s">
-        <v>67</v>
-      </c>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="13"/>
+      <c r="B33" s="12"/>
       <c r="C33" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="15"/>
-      <c r="B34" s="14"/>
+      <c r="A34" s="13"/>
+      <c r="B34" s="12"/>
       <c r="C34" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="15"/>
-      <c r="B35" s="14"/>
+      <c r="A35" s="13"/>
+      <c r="B35" s="12"/>
       <c r="C35" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="15"/>
-      <c r="B36" s="14"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A36" s="13">
+        <v>7</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>76</v>
+      </c>
       <c r="C36" s="1" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A37" s="15">
-        <v>7</v>
-      </c>
-      <c r="B37" s="14" t="s">
-        <v>76</v>
-      </c>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="13"/>
+      <c r="B37" s="12"/>
       <c r="C37" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="15"/>
-      <c r="B38" s="14"/>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A38" s="13"/>
+      <c r="B38" s="12"/>
       <c r="C38" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A39" s="15"/>
-      <c r="B39" s="14"/>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="13"/>
+      <c r="B39" s="12"/>
       <c r="C39" s="1" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="15"/>
-      <c r="B40" s="14"/>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" s="13">
+        <v>8</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>85</v>
+      </c>
       <c r="C40" s="1" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A41" s="15">
-        <v>8</v>
-      </c>
-      <c r="B41" s="14" t="s">
-        <v>85</v>
-      </c>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="13"/>
+      <c r="B41" s="12"/>
       <c r="C41" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="15"/>
-      <c r="B42" s="14"/>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>9</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>90</v>
+      </c>
       <c r="C42" s="1" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A43" s="2">
-        <v>9</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>90</v>
+      <c r="A43" s="13">
+        <v>10</v>
+      </c>
+      <c r="B43" s="12" t="s">
+        <v>93</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A44" s="15">
-        <v>10</v>
-      </c>
-      <c r="B44" s="14" t="s">
-        <v>93</v>
-      </c>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="13"/>
+      <c r="B44" s="12"/>
       <c r="C44" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="15"/>
-      <c r="B45" s="14"/>
-      <c r="C45" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D45" s="1" t="s">
         <v>97</v>
       </c>
     </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="13"/>
+      <c r="B45" s="12"/>
+    </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="15"/>
-      <c r="B46" s="14"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="15"/>
-      <c r="B47" s="14"/>
+      <c r="A46" s="13"/>
+      <c r="B46" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="18">
     <mergeCell ref="A2:A11"/>
-    <mergeCell ref="B13:B17"/>
-    <mergeCell ref="A13:A17"/>
-    <mergeCell ref="B2:B12"/>
-    <mergeCell ref="A18:A22"/>
-    <mergeCell ref="B18:B22"/>
-    <mergeCell ref="B23:B28"/>
-    <mergeCell ref="A23:A28"/>
-    <mergeCell ref="B29:B32"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="B33:B36"/>
-    <mergeCell ref="A33:A36"/>
-    <mergeCell ref="B44:B47"/>
-    <mergeCell ref="A44:A47"/>
-    <mergeCell ref="B37:B40"/>
-    <mergeCell ref="A37:A40"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B12:B16"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="B2:B11"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="B17:B21"/>
+    <mergeCell ref="B22:B27"/>
+    <mergeCell ref="A22:A27"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="B32:B35"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="B43:B46"/>
+    <mergeCell ref="A43:A46"/>
+    <mergeCell ref="B36:B39"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="A40:A41"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
NC-1.11 - Estrutura inicial com repositórios genéricos + services genéricos + mapper genérico
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\AppNotificacoesCrimesCidade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{390FDE29-3C40-4ADE-A615-B21B70A2AB0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95CDA426-B28B-44EF-A4AF-D7C65C0FE533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{996D4097-5510-4348-97EC-A204A307EBA8}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="106">
   <si>
     <t>Descrição</t>
   </si>
@@ -351,6 +351,12 @@
   </si>
   <si>
     <t>Passar para o backend a rotina de pesquisa de endereço</t>
+  </si>
+  <si>
+    <t>1.11</t>
+  </si>
+  <si>
+    <t>Criar estrutura inicial do backend com repositórios genéricos e unitOfWork e métodos assincronos</t>
   </si>
 </sst>
 </file>
@@ -438,10 +444,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -777,10 +783,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94151779-DED3-44C5-B19B-FEA501E890E9}">
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -809,10 +815,10 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13">
+      <c r="A2" s="12">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="13" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -826,8 +832,8 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="B3" s="12"/>
+      <c r="A3" s="12"/>
+      <c r="B3" s="13"/>
       <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
@@ -839,8 +845,8 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
-      <c r="B4" s="12"/>
+      <c r="A4" s="12"/>
+      <c r="B4" s="13"/>
       <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
@@ -852,8 +858,8 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-      <c r="B5" s="12"/>
+      <c r="A5" s="12"/>
+      <c r="B5" s="13"/>
       <c r="C5" s="4" t="s">
         <v>8</v>
       </c>
@@ -865,8 +871,8 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
-      <c r="B6" s="12"/>
+      <c r="A6" s="12"/>
+      <c r="B6" s="13"/>
       <c r="C6" s="4" t="s">
         <v>9</v>
       </c>
@@ -878,8 +884,8 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
-      <c r="B7" s="12"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="13"/>
       <c r="C7" s="4" t="s">
         <v>10</v>
       </c>
@@ -891,8 +897,8 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="12"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="13"/>
       <c r="C8" s="6" t="s">
         <v>11</v>
       </c>
@@ -904,8 +910,8 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="12"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="13"/>
       <c r="C9" s="4" t="s">
         <v>12</v>
       </c>
@@ -917,21 +923,21 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="8" t="s">
+      <c r="A10" s="12"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="9" t="s">
-        <v>101</v>
+      <c r="E10" s="5" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-      <c r="B11" s="12"/>
+      <c r="A11" s="12"/>
+      <c r="B11" s="13"/>
       <c r="C11" s="4" t="s">
         <v>98</v>
       </c>
@@ -942,422 +948,435 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="13">
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="12"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="12">
         <v>2</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B13" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C13" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D13" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="1" t="s">
+      <c r="E13" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="12"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="4" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="12"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D15" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="1" t="s">
+      <c r="E15" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="12"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="1" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="12"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="13">
+    <row r="18" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="12">
         <v>3</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B18" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C18" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D18" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="E17" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="1" t="s">
+      <c r="E18" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="12"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="1" t="s">
+    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="12"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="4" t="s">
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="12"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D21" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E20" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="10" t="s">
+      <c r="E21" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="12"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="D22" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="E21" s="11"/>
-    </row>
-    <row r="22" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="13">
+      <c r="E22" s="11"/>
+    </row>
+    <row r="23" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="12">
         <v>4</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B23" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C23" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D23" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E22" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="13"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="1" t="s">
+      <c r="E23" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="12"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D24" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="13"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="4" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="12"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D25" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E24" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="13"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="1" t="s">
+      <c r="E25" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="12"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="13"/>
-      <c r="B26" s="12"/>
-      <c r="C26" s="4" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="12"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D27" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E26" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="13"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="1" t="s">
+      <c r="E27" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="12"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="13">
+    <row r="29" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="12">
         <v>5</v>
       </c>
-      <c r="B28" s="12" t="s">
+      <c r="B29" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D29" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="13"/>
-      <c r="B29" s="12"/>
-      <c r="C29" s="1" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="12"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D30" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="13"/>
-      <c r="B30" s="12"/>
-      <c r="C30" s="1" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="12"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D31" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="13"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="1" t="s">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="12"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D32" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="13">
-        <v>6</v>
-      </c>
-      <c r="B32" s="12" t="s">
+    <row r="33" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="12">
+        <v>6</v>
+      </c>
+      <c r="B33" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D33" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="13"/>
-      <c r="B33" s="12"/>
-      <c r="C33" s="1" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="12"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D34" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="13"/>
-      <c r="B34" s="12"/>
-      <c r="C34" s="1" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="12"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="13"/>
-      <c r="B35" s="12"/>
-      <c r="C35" s="1" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="12"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D36" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A36" s="13">
+    <row r="37" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A37" s="12">
         <v>7</v>
       </c>
-      <c r="B36" s="12" t="s">
+      <c r="B37" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C37" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D37" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="13"/>
-      <c r="B37" s="12"/>
-      <c r="C37" s="1" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="12"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D38" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A38" s="13"/>
-      <c r="B38" s="12"/>
-      <c r="C38" s="1" t="s">
+    <row r="39" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A39" s="12"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D39" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="13"/>
-      <c r="B39" s="12"/>
-      <c r="C39" s="1" t="s">
+    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="12"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D40" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A40" s="13">
+    <row r="41" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A41" s="12">
         <v>8</v>
       </c>
-      <c r="B40" s="12" t="s">
+      <c r="B41" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C41" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="D41" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="13"/>
-      <c r="B41" s="12"/>
-      <c r="C41" s="1" t="s">
+    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="12"/>
+      <c r="B42" s="13"/>
+      <c r="C42" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="D42" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A42" s="2">
+    <row r="43" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
         <v>9</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B43" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C43" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D43" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A43" s="13">
+    <row r="44" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A44" s="12">
         <v>10</v>
       </c>
-      <c r="B43" s="12" t="s">
+      <c r="B44" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C44" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D44" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="13"/>
-      <c r="B44" s="12"/>
-      <c r="C44" s="1" t="s">
+    <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="12"/>
+      <c r="B45" s="13"/>
+      <c r="C45" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="D45" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="13"/>
-      <c r="B45" s="12"/>
-    </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="13"/>
-      <c r="B46" s="12"/>
+      <c r="A46" s="12"/>
+      <c r="B46" s="13"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="12"/>
+      <c r="B47" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A2:A11"/>
-    <mergeCell ref="B12:B16"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="B2:B11"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="B17:B21"/>
-    <mergeCell ref="B22:B27"/>
-    <mergeCell ref="A22:A27"/>
-    <mergeCell ref="B28:B31"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="B32:B35"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="B43:B46"/>
-    <mergeCell ref="A43:A46"/>
-    <mergeCell ref="B36:B39"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="B44:B47"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="B37:B40"/>
+    <mergeCell ref="A37:A40"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B23:B28"/>
+    <mergeCell ref="A23:A28"/>
+    <mergeCell ref="B29:B32"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="B33:B36"/>
+    <mergeCell ref="A33:A36"/>
+    <mergeCell ref="B13:B17"/>
+    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="A18:A22"/>
+    <mergeCell ref="B18:B22"/>
+    <mergeCell ref="A2:A12"/>
+    <mergeCell ref="B2:B12"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Remoção de arquivos que não vão ser versionados
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\AppNotificacoesCrimesCidade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95CDA426-B28B-44EF-A4AF-D7C65C0FE533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{732CE144-3AF5-4443-9EF5-B38D980831E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{996D4097-5510-4348-97EC-A204A307EBA8}"/>
   </bookViews>
@@ -444,10 +444,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -785,8 +785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94151779-DED3-44C5-B19B-FEA501E890E9}">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -815,10 +815,10 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12">
+      <c r="A2" s="13">
         <v>1</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -832,8 +832,8 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
-      <c r="B3" s="13"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="12"/>
       <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
@@ -845,8 +845,8 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="13"/>
+      <c r="A4" s="13"/>
+      <c r="B4" s="12"/>
       <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
@@ -858,8 +858,8 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
-      <c r="B5" s="13"/>
+      <c r="A5" s="13"/>
+      <c r="B5" s="12"/>
       <c r="C5" s="4" t="s">
         <v>8</v>
       </c>
@@ -871,8 +871,8 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
-      <c r="B6" s="13"/>
+      <c r="A6" s="13"/>
+      <c r="B6" s="12"/>
       <c r="C6" s="4" t="s">
         <v>9</v>
       </c>
@@ -884,8 +884,8 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
-      <c r="B7" s="13"/>
+      <c r="A7" s="13"/>
+      <c r="B7" s="12"/>
       <c r="C7" s="4" t="s">
         <v>10</v>
       </c>
@@ -897,8 +897,8 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
-      <c r="B8" s="13"/>
+      <c r="A8" s="13"/>
+      <c r="B8" s="12"/>
       <c r="C8" s="6" t="s">
         <v>11</v>
       </c>
@@ -910,8 +910,8 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
-      <c r="B9" s="13"/>
+      <c r="A9" s="13"/>
+      <c r="B9" s="12"/>
       <c r="C9" s="4" t="s">
         <v>12</v>
       </c>
@@ -923,8 +923,8 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
-      <c r="B10" s="13"/>
+      <c r="A10" s="13"/>
+      <c r="B10" s="12"/>
       <c r="C10" s="4" t="s">
         <v>13</v>
       </c>
@@ -936,8 +936,8 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
-      <c r="B11" s="13"/>
+      <c r="A11" s="13"/>
+      <c r="B11" s="12"/>
       <c r="C11" s="4" t="s">
         <v>98</v>
       </c>
@@ -949,8 +949,8 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-      <c r="B12" s="13"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="12"/>
       <c r="C12" s="8" t="s">
         <v>105</v>
       </c>
@@ -962,10 +962,10 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="12">
+      <c r="A13" s="13">
         <v>2</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="12" t="s">
         <v>25</v>
       </c>
       <c r="C13" s="4" t="s">
@@ -979,8 +979,8 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
-      <c r="B14" s="13"/>
+      <c r="A14" s="13"/>
+      <c r="B14" s="12"/>
       <c r="C14" s="1" t="s">
         <v>27</v>
       </c>
@@ -989,8 +989,8 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
-      <c r="B15" s="13"/>
+      <c r="A15" s="13"/>
+      <c r="B15" s="12"/>
       <c r="C15" s="4" t="s">
         <v>28</v>
       </c>
@@ -1002,8 +1002,8 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
-      <c r="B16" s="13"/>
+      <c r="A16" s="13"/>
+      <c r="B16" s="12"/>
       <c r="C16" s="1" t="s">
         <v>29</v>
       </c>
@@ -1012,8 +1012,8 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
-      <c r="B17" s="13"/>
+      <c r="A17" s="13"/>
+      <c r="B17" s="12"/>
       <c r="C17" s="1" t="s">
         <v>30</v>
       </c>
@@ -1022,10 +1022,10 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="12">
+      <c r="A18" s="13">
         <v>3</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="12" t="s">
         <v>36</v>
       </c>
       <c r="C18" s="4" t="s">
@@ -1039,8 +1039,8 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
-      <c r="B19" s="13"/>
+      <c r="A19" s="13"/>
+      <c r="B19" s="12"/>
       <c r="C19" s="1" t="s">
         <v>38</v>
       </c>
@@ -1049,8 +1049,8 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="12"/>
-      <c r="B20" s="13"/>
+      <c r="A20" s="13"/>
+      <c r="B20" s="12"/>
       <c r="C20" s="1" t="s">
         <v>39</v>
       </c>
@@ -1059,8 +1059,8 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="12"/>
-      <c r="B21" s="13"/>
+      <c r="A21" s="13"/>
+      <c r="B21" s="12"/>
       <c r="C21" s="4" t="s">
         <v>40</v>
       </c>
@@ -1072,8 +1072,8 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="12"/>
-      <c r="B22" s="13"/>
+      <c r="A22" s="13"/>
+      <c r="B22" s="12"/>
       <c r="C22" s="10" t="s">
         <v>103</v>
       </c>
@@ -1083,10 +1083,10 @@
       <c r="E22" s="11"/>
     </row>
     <row r="23" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="12">
+      <c r="A23" s="13">
         <v>4</v>
       </c>
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="12" t="s">
         <v>45</v>
       </c>
       <c r="C23" s="4" t="s">
@@ -1100,8 +1100,8 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="12"/>
-      <c r="B24" s="13"/>
+      <c r="A24" s="13"/>
+      <c r="B24" s="12"/>
       <c r="C24" s="1" t="s">
         <v>47</v>
       </c>
@@ -1110,8 +1110,8 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="12"/>
-      <c r="B25" s="13"/>
+      <c r="A25" s="13"/>
+      <c r="B25" s="12"/>
       <c r="C25" s="4" t="s">
         <v>48</v>
       </c>
@@ -1123,8 +1123,8 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="12"/>
-      <c r="B26" s="13"/>
+      <c r="A26" s="13"/>
+      <c r="B26" s="12"/>
       <c r="C26" s="1" t="s">
         <v>49</v>
       </c>
@@ -1133,8 +1133,8 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="12"/>
-      <c r="B27" s="13"/>
+      <c r="A27" s="13"/>
+      <c r="B27" s="12"/>
       <c r="C27" s="4" t="s">
         <v>50</v>
       </c>
@@ -1146,8 +1146,8 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="12"/>
-      <c r="B28" s="13"/>
+      <c r="A28" s="13"/>
+      <c r="B28" s="12"/>
       <c r="C28" s="1" t="s">
         <v>51</v>
       </c>
@@ -1156,10 +1156,10 @@
       </c>
     </row>
     <row r="29" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="12">
+      <c r="A29" s="13">
         <v>5</v>
       </c>
-      <c r="B29" s="13" t="s">
+      <c r="B29" s="12" t="s">
         <v>58</v>
       </c>
       <c r="C29" s="1" t="s">
@@ -1170,8 +1170,8 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="12"/>
-      <c r="B30" s="13"/>
+      <c r="A30" s="13"/>
+      <c r="B30" s="12"/>
       <c r="C30" s="1" t="s">
         <v>60</v>
       </c>
@@ -1180,8 +1180,8 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="12"/>
-      <c r="B31" s="13"/>
+      <c r="A31" s="13"/>
+      <c r="B31" s="12"/>
       <c r="C31" s="1" t="s">
         <v>61</v>
       </c>
@@ -1190,8 +1190,8 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="12"/>
-      <c r="B32" s="13"/>
+      <c r="A32" s="13"/>
+      <c r="B32" s="12"/>
       <c r="C32" s="1" t="s">
         <v>62</v>
       </c>
@@ -1200,10 +1200,10 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="12">
-        <v>6</v>
-      </c>
-      <c r="B33" s="13" t="s">
+      <c r="A33" s="13">
+        <v>6</v>
+      </c>
+      <c r="B33" s="12" t="s">
         <v>67</v>
       </c>
       <c r="C33" s="1" t="s">
@@ -1214,8 +1214,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="12"/>
-      <c r="B34" s="13"/>
+      <c r="A34" s="13"/>
+      <c r="B34" s="12"/>
       <c r="C34" s="1" t="s">
         <v>69</v>
       </c>
@@ -1224,8 +1224,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="12"/>
-      <c r="B35" s="13"/>
+      <c r="A35" s="13"/>
+      <c r="B35" s="12"/>
       <c r="C35" s="1" t="s">
         <v>70</v>
       </c>
@@ -1234,8 +1234,8 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="12"/>
-      <c r="B36" s="13"/>
+      <c r="A36" s="13"/>
+      <c r="B36" s="12"/>
       <c r="C36" s="1" t="s">
         <v>71</v>
       </c>
@@ -1244,10 +1244,10 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A37" s="12">
+      <c r="A37" s="13">
         <v>7</v>
       </c>
-      <c r="B37" s="13" t="s">
+      <c r="B37" s="12" t="s">
         <v>76</v>
       </c>
       <c r="C37" s="1" t="s">
@@ -1258,8 +1258,8 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="12"/>
-      <c r="B38" s="13"/>
+      <c r="A38" s="13"/>
+      <c r="B38" s="12"/>
       <c r="C38" s="1" t="s">
         <v>77</v>
       </c>
@@ -1268,8 +1268,8 @@
       </c>
     </row>
     <row r="39" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A39" s="12"/>
-      <c r="B39" s="13"/>
+      <c r="A39" s="13"/>
+      <c r="B39" s="12"/>
       <c r="C39" s="1" t="s">
         <v>79</v>
       </c>
@@ -1278,8 +1278,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="12"/>
-      <c r="B40" s="13"/>
+      <c r="A40" s="13"/>
+      <c r="B40" s="12"/>
       <c r="C40" s="1" t="s">
         <v>83</v>
       </c>
@@ -1288,10 +1288,10 @@
       </c>
     </row>
     <row r="41" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A41" s="12">
+      <c r="A41" s="13">
         <v>8</v>
       </c>
-      <c r="B41" s="13" t="s">
+      <c r="B41" s="12" t="s">
         <v>85</v>
       </c>
       <c r="C41" s="1" t="s">
@@ -1302,8 +1302,8 @@
       </c>
     </row>
     <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="12"/>
-      <c r="B42" s="13"/>
+      <c r="A42" s="13"/>
+      <c r="B42" s="12"/>
       <c r="C42" s="1" t="s">
         <v>87</v>
       </c>
@@ -1326,10 +1326,10 @@
       </c>
     </row>
     <row r="44" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A44" s="12">
+      <c r="A44" s="13">
         <v>10</v>
       </c>
-      <c r="B44" s="13" t="s">
+      <c r="B44" s="12" t="s">
         <v>93</v>
       </c>
       <c r="C44" s="1" t="s">
@@ -1340,8 +1340,8 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="12"/>
-      <c r="B45" s="13"/>
+      <c r="A45" s="13"/>
+      <c r="B45" s="12"/>
       <c r="C45" s="1" t="s">
         <v>95</v>
       </c>
@@ -1350,33 +1350,33 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="12"/>
-      <c r="B46" s="13"/>
+      <c r="A46" s="13"/>
+      <c r="B46" s="12"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="12"/>
-      <c r="B47" s="13"/>
+      <c r="A47" s="13"/>
+      <c r="B47" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B13:B17"/>
+    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="A18:A22"/>
+    <mergeCell ref="B18:B22"/>
+    <mergeCell ref="A2:A12"/>
+    <mergeCell ref="B2:B12"/>
+    <mergeCell ref="B23:B28"/>
+    <mergeCell ref="A23:A28"/>
+    <mergeCell ref="B29:B32"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="B33:B36"/>
+    <mergeCell ref="A33:A36"/>
     <mergeCell ref="B44:B47"/>
     <mergeCell ref="A44:A47"/>
     <mergeCell ref="B37:B40"/>
     <mergeCell ref="A37:A40"/>
     <mergeCell ref="B41:B42"/>
     <mergeCell ref="A41:A42"/>
-    <mergeCell ref="B23:B28"/>
-    <mergeCell ref="A23:A28"/>
-    <mergeCell ref="B29:B32"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="B33:B36"/>
-    <mergeCell ref="A33:A36"/>
-    <mergeCell ref="B13:B17"/>
-    <mergeCell ref="A13:A17"/>
-    <mergeCell ref="A18:A22"/>
-    <mergeCell ref="B18:B22"/>
-    <mergeCell ref="A2:A12"/>
-    <mergeCell ref="B2:B12"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
NC-4.2 - Rotina para salvar as ocorrências de assalto
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\AppNotificacoesCrimesCidade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{732CE144-3AF5-4443-9EF5-B38D980831E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD59E59F-6401-4DCE-88FD-7BCC155B8089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{996D4097-5510-4348-97EC-A204A307EBA8}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="106">
   <si>
     <t>Descrição</t>
   </si>
@@ -786,7 +786,7 @@
   <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -951,14 +951,14 @@
     <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
       <c r="B12" s="12"/>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="E12" s="9" t="s">
-        <v>101</v>
+      <c r="E12" s="5" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1102,11 +1102,14 @@
     <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="13"/>
       <c r="B24" s="12"/>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" s="8" t="s">
         <v>53</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1359,24 +1362,24 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B44:B47"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="B37:B40"/>
+    <mergeCell ref="A37:A40"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B23:B28"/>
+    <mergeCell ref="A23:A28"/>
+    <mergeCell ref="B29:B32"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="B33:B36"/>
+    <mergeCell ref="A33:A36"/>
     <mergeCell ref="B13:B17"/>
     <mergeCell ref="A13:A17"/>
     <mergeCell ref="A18:A22"/>
     <mergeCell ref="B18:B22"/>
     <mergeCell ref="A2:A12"/>
     <mergeCell ref="B2:B12"/>
-    <mergeCell ref="B23:B28"/>
-    <mergeCell ref="A23:A28"/>
-    <mergeCell ref="B29:B32"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="B33:B36"/>
-    <mergeCell ref="A33:A36"/>
-    <mergeCell ref="B44:B47"/>
-    <mergeCell ref="A44:A47"/>
-    <mergeCell ref="B37:B40"/>
-    <mergeCell ref="A37:A40"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="A41:A42"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
NC-4.2 - Desenvolvimento da rotina de cadastro de ocorrências de roubo + integração com front
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\AppNotificacoesCrimesCidade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD59E59F-6401-4DCE-88FD-7BCC155B8089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C7D673-7F5F-4365-A3A9-1D0123A0FC58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{996D4097-5510-4348-97EC-A204A307EBA8}"/>
+    <workbookView xWindow="15240" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{996D4097-5510-4348-97EC-A204A307EBA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="106">
   <si>
     <t>Descrição</t>
   </si>
@@ -785,8 +785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94151779-DED3-44C5-B19B-FEA501E890E9}">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1102,14 +1102,14 @@
     <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="13"/>
       <c r="B24" s="12"/>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E24" s="9" t="s">
-        <v>101</v>
+      <c r="E24" s="5" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1128,11 +1128,14 @@
     <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="13"/>
       <c r="B26" s="12"/>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D26" s="8" t="s">
         <v>55</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1362,24 +1365,24 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B13:B17"/>
+    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="A18:A22"/>
+    <mergeCell ref="B18:B22"/>
+    <mergeCell ref="A2:A12"/>
+    <mergeCell ref="B2:B12"/>
+    <mergeCell ref="B23:B28"/>
+    <mergeCell ref="A23:A28"/>
+    <mergeCell ref="B29:B32"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="B33:B36"/>
+    <mergeCell ref="A33:A36"/>
     <mergeCell ref="B44:B47"/>
     <mergeCell ref="A44:A47"/>
     <mergeCell ref="B37:B40"/>
     <mergeCell ref="A37:A40"/>
     <mergeCell ref="B41:B42"/>
     <mergeCell ref="A41:A42"/>
-    <mergeCell ref="B23:B28"/>
-    <mergeCell ref="A23:A28"/>
-    <mergeCell ref="B29:B32"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="B33:B36"/>
-    <mergeCell ref="A33:A36"/>
-    <mergeCell ref="B13:B17"/>
-    <mergeCell ref="A13:A17"/>
-    <mergeCell ref="A18:A22"/>
-    <mergeCell ref="B18:B22"/>
-    <mergeCell ref="A2:A12"/>
-    <mergeCell ref="B2:B12"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
NC-4.6 - Desenvolvimento da rotina de criação de ocorrências de agressão + integração com front
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\AppNotificacoesCrimesCidade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C7D673-7F5F-4365-A3A9-1D0123A0FC58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BEBFCC1-4246-4853-8AA5-D95B08CDC369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15240" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{996D4097-5510-4348-97EC-A204A307EBA8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{996D4097-5510-4348-97EC-A204A307EBA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="106">
   <si>
     <t>Descrição</t>
   </si>
@@ -786,7 +786,7 @@
   <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1128,14 +1128,14 @@
     <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="13"/>
       <c r="B26" s="12"/>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E26" s="9" t="s">
-        <v>101</v>
+      <c r="E26" s="5" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1154,11 +1154,14 @@
     <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="13"/>
       <c r="B28" s="12"/>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D28" s="8" t="s">
         <v>57</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1365,24 +1368,24 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B44:B47"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="B37:B40"/>
+    <mergeCell ref="A37:A40"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B23:B28"/>
+    <mergeCell ref="A23:A28"/>
+    <mergeCell ref="B29:B32"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="B33:B36"/>
+    <mergeCell ref="A33:A36"/>
     <mergeCell ref="B13:B17"/>
     <mergeCell ref="A13:A17"/>
     <mergeCell ref="A18:A22"/>
     <mergeCell ref="B18:B22"/>
     <mergeCell ref="A2:A12"/>
     <mergeCell ref="B2:B12"/>
-    <mergeCell ref="B23:B28"/>
-    <mergeCell ref="A23:A28"/>
-    <mergeCell ref="B29:B32"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="B33:B36"/>
-    <mergeCell ref="A33:A36"/>
-    <mergeCell ref="B44:B47"/>
-    <mergeCell ref="A44:A47"/>
-    <mergeCell ref="B37:B40"/>
-    <mergeCell ref="A37:A40"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="A41:A42"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
NC-3.2-3.3 - Rotina para retornar todos os crimes com filtro de datas + Plotar no app as ocorrências nas localizações onde ocorreram
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\AppNotificacoesCrimesCidade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BEBFCC1-4246-4853-8AA5-D95B08CDC369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4540C4CE-A08E-4AFC-934B-28268157CA92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{996D4097-5510-4348-97EC-A204A307EBA8}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="108">
   <si>
     <t>Descrição</t>
   </si>
@@ -344,9 +344,6 @@
     <t>A definir</t>
   </si>
   <si>
-    <t>Fazendo</t>
-  </si>
-  <si>
     <t>3.5</t>
   </si>
   <si>
@@ -357,6 +354,15 @@
   </si>
   <si>
     <t>Criar estrutura inicial do backend com repositórios genéricos e unitOfWork e métodos assincronos</t>
+  </si>
+  <si>
+    <t>Criar rotina no backend para cadastro da ocorrência outros</t>
+  </si>
+  <si>
+    <t>4.7</t>
+  </si>
+  <si>
+    <t>Concluido</t>
   </si>
 </sst>
 </file>
@@ -378,7 +384,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -397,12 +403,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -416,7 +416,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -435,10 +435,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -783,10 +779,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94151779-DED3-44C5-B19B-FEA501E890E9}">
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38:B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -815,10 +811,10 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13">
+      <c r="A2" s="11">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="10" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -832,8 +828,8 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="B3" s="12"/>
+      <c r="A3" s="11"/>
+      <c r="B3" s="10"/>
       <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
@@ -845,8 +841,8 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
-      <c r="B4" s="12"/>
+      <c r="A4" s="11"/>
+      <c r="B4" s="10"/>
       <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
@@ -858,8 +854,8 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-      <c r="B5" s="12"/>
+      <c r="A5" s="11"/>
+      <c r="B5" s="10"/>
       <c r="C5" s="4" t="s">
         <v>8</v>
       </c>
@@ -871,8 +867,8 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
-      <c r="B6" s="12"/>
+      <c r="A6" s="11"/>
+      <c r="B6" s="10"/>
       <c r="C6" s="4" t="s">
         <v>9</v>
       </c>
@@ -884,8 +880,8 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
-      <c r="B7" s="12"/>
+      <c r="A7" s="11"/>
+      <c r="B7" s="10"/>
       <c r="C7" s="4" t="s">
         <v>10</v>
       </c>
@@ -897,8 +893,8 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="12"/>
+      <c r="A8" s="11"/>
+      <c r="B8" s="10"/>
       <c r="C8" s="6" t="s">
         <v>11</v>
       </c>
@@ -910,8 +906,8 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="12"/>
+      <c r="A9" s="11"/>
+      <c r="B9" s="10"/>
       <c r="C9" s="4" t="s">
         <v>12</v>
       </c>
@@ -923,8 +919,8 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-      <c r="B10" s="12"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="10"/>
       <c r="C10" s="4" t="s">
         <v>13</v>
       </c>
@@ -936,8 +932,8 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-      <c r="B11" s="12"/>
+      <c r="A11" s="11"/>
+      <c r="B11" s="10"/>
       <c r="C11" s="4" t="s">
         <v>98</v>
       </c>
@@ -949,23 +945,23 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
-      <c r="B12" s="12"/>
+      <c r="A12" s="11"/>
+      <c r="B12" s="10"/>
       <c r="C12" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="13">
+      <c r="A13" s="11">
         <v>2</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="10" t="s">
         <v>25</v>
       </c>
       <c r="C13" s="4" t="s">
@@ -979,8 +975,8 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
-      <c r="B14" s="12"/>
+      <c r="A14" s="11"/>
+      <c r="B14" s="10"/>
       <c r="C14" s="1" t="s">
         <v>27</v>
       </c>
@@ -989,8 +985,8 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
-      <c r="B15" s="12"/>
+      <c r="A15" s="11"/>
+      <c r="B15" s="10"/>
       <c r="C15" s="4" t="s">
         <v>28</v>
       </c>
@@ -1002,8 +998,8 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
-      <c r="B16" s="12"/>
+      <c r="A16" s="11"/>
+      <c r="B16" s="10"/>
       <c r="C16" s="1" t="s">
         <v>29</v>
       </c>
@@ -1012,8 +1008,8 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
-      <c r="B17" s="12"/>
+      <c r="A17" s="11"/>
+      <c r="B17" s="10"/>
       <c r="C17" s="1" t="s">
         <v>30</v>
       </c>
@@ -1022,10 +1018,10 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="13">
+      <c r="A18" s="11">
         <v>3</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="10" t="s">
         <v>36</v>
       </c>
       <c r="C18" s="4" t="s">
@@ -1039,28 +1035,34 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="1" t="s">
+      <c r="A19" s="11"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="4" t="s">
         <v>42</v>
       </c>
+      <c r="E19" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="1" t="s">
+      <c r="A20" s="11"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="4" t="s">
         <v>43</v>
       </c>
+      <c r="E20" s="5" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
-      <c r="B21" s="12"/>
+      <c r="A21" s="11"/>
+      <c r="B21" s="10"/>
       <c r="C21" s="4" t="s">
         <v>40</v>
       </c>
@@ -1072,21 +1074,21 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="13"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="D22" s="10" t="s">
+      <c r="A22" s="11"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="E22" s="11"/>
+      <c r="D22" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="E22" s="9"/>
     </row>
     <row r="23" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="13">
+      <c r="A23" s="11">
         <v>4</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="10" t="s">
         <v>45</v>
       </c>
       <c r="C23" s="4" t="s">
@@ -1100,8 +1102,8 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="13"/>
-      <c r="B24" s="12"/>
+      <c r="A24" s="11"/>
+      <c r="B24" s="10"/>
       <c r="C24" s="4" t="s">
         <v>47</v>
       </c>
@@ -1113,8 +1115,8 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="13"/>
-      <c r="B25" s="12"/>
+      <c r="A25" s="11"/>
+      <c r="B25" s="10"/>
       <c r="C25" s="4" t="s">
         <v>48</v>
       </c>
@@ -1126,8 +1128,8 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="13"/>
-      <c r="B26" s="12"/>
+      <c r="A26" s="11"/>
+      <c r="B26" s="10"/>
       <c r="C26" s="4" t="s">
         <v>49</v>
       </c>
@@ -1139,8 +1141,8 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="13"/>
-      <c r="B27" s="12"/>
+      <c r="A27" s="11"/>
+      <c r="B27" s="10"/>
       <c r="C27" s="4" t="s">
         <v>50</v>
       </c>
@@ -1152,234 +1154,245 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="13"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="8" t="s">
+      <c r="A28" s="11"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="D28" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="E28" s="9" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="13">
+      <c r="E28" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="11"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="E29" s="9"/>
+    </row>
+    <row r="30" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="11">
         <v>5</v>
       </c>
-      <c r="B29" s="12" t="s">
+      <c r="B30" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D30" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="13"/>
-      <c r="B30" s="12"/>
-      <c r="C30" s="1" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="11"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D31" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="13"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="1" t="s">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="11"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D32" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="13"/>
-      <c r="B32" s="12"/>
-      <c r="C32" s="1" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="11"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D33" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="13">
-        <v>6</v>
-      </c>
-      <c r="B33" s="12" t="s">
+    <row r="34" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="11">
+        <v>6</v>
+      </c>
+      <c r="B34" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D34" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="13"/>
-      <c r="B34" s="12"/>
-      <c r="C34" s="1" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="11"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="13"/>
-      <c r="B35" s="12"/>
-      <c r="C35" s="1" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="11"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D36" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="13"/>
-      <c r="B36" s="12"/>
-      <c r="C36" s="1" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="11"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D37" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A37" s="13">
+    <row r="38" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A38" s="11">
         <v>7</v>
       </c>
-      <c r="B37" s="12" t="s">
+      <c r="B38" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C38" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D38" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="13"/>
-      <c r="B38" s="12"/>
-      <c r="C38" s="1" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="11"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D39" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A39" s="13"/>
-      <c r="B39" s="12"/>
-      <c r="C39" s="1" t="s">
+    <row r="40" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A40" s="11"/>
+      <c r="B40" s="10"/>
+      <c r="C40" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D40" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="13"/>
-      <c r="B40" s="12"/>
-      <c r="C40" s="1" t="s">
+    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="11"/>
+      <c r="B41" s="10"/>
+      <c r="C41" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="D41" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A41" s="13">
+    <row r="42" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A42" s="11">
         <v>8</v>
       </c>
-      <c r="B41" s="12" t="s">
+      <c r="B42" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C42" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="D42" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="13"/>
-      <c r="B42" s="12"/>
-      <c r="C42" s="1" t="s">
+    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="11"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D43" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A43" s="2">
+    <row r="44" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
         <v>9</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B44" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C44" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D44" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A44" s="13">
+    <row r="45" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A45" s="11">
         <v>10</v>
       </c>
-      <c r="B44" s="12" t="s">
+      <c r="B45" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C45" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="D45" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="13"/>
-      <c r="B45" s="12"/>
-      <c r="C45" s="1" t="s">
+    <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="11"/>
+      <c r="B46" s="10"/>
+      <c r="C46" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D46" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="13"/>
-      <c r="B46" s="12"/>
-    </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="13"/>
-      <c r="B47" s="12"/>
+      <c r="A47" s="11"/>
+      <c r="B47" s="10"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="11"/>
+      <c r="B48" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B44:B47"/>
-    <mergeCell ref="A44:A47"/>
-    <mergeCell ref="B37:B40"/>
-    <mergeCell ref="A37:A40"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="B23:B28"/>
-    <mergeCell ref="A23:A28"/>
-    <mergeCell ref="B29:B32"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="B33:B36"/>
-    <mergeCell ref="A33:A36"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="B23:B29"/>
+    <mergeCell ref="A23:A29"/>
     <mergeCell ref="B13:B17"/>
     <mergeCell ref="A13:A17"/>
     <mergeCell ref="A18:A22"/>

</xml_diff>

<commit_message>
NC-2.2 Rotina delogin no backend e integração com o front-End
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\AppNotificacoesCrimesCidade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4540C4CE-A08E-4AFC-934B-28268157CA92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67B3763E-80DF-4F50-844E-DEF691198089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{996D4097-5510-4348-97EC-A204A307EBA8}"/>
   </bookViews>
@@ -384,7 +384,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -403,6 +403,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -416,7 +422,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -439,6 +445,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -781,8 +791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94151779-DED3-44C5-B19B-FEA501E890E9}">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38:B41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="C14:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -811,10 +821,10 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11">
+      <c r="A2" s="13">
         <v>1</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="12" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -828,8 +838,8 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="10"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="12"/>
       <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
@@ -841,8 +851,8 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="10"/>
+      <c r="A4" s="13"/>
+      <c r="B4" s="12"/>
       <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
@@ -854,8 +864,8 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="10"/>
+      <c r="A5" s="13"/>
+      <c r="B5" s="12"/>
       <c r="C5" s="4" t="s">
         <v>8</v>
       </c>
@@ -867,8 +877,8 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="10"/>
+      <c r="A6" s="13"/>
+      <c r="B6" s="12"/>
       <c r="C6" s="4" t="s">
         <v>9</v>
       </c>
@@ -880,8 +890,8 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="10"/>
+      <c r="A7" s="13"/>
+      <c r="B7" s="12"/>
       <c r="C7" s="4" t="s">
         <v>10</v>
       </c>
@@ -893,8 +903,8 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
-      <c r="B8" s="10"/>
+      <c r="A8" s="13"/>
+      <c r="B8" s="12"/>
       <c r="C8" s="6" t="s">
         <v>11</v>
       </c>
@@ -906,8 +916,8 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
-      <c r="B9" s="10"/>
+      <c r="A9" s="13"/>
+      <c r="B9" s="12"/>
       <c r="C9" s="4" t="s">
         <v>12</v>
       </c>
@@ -919,8 +929,8 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
-      <c r="B10" s="10"/>
+      <c r="A10" s="13"/>
+      <c r="B10" s="12"/>
       <c r="C10" s="4" t="s">
         <v>13</v>
       </c>
@@ -932,8 +942,8 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
-      <c r="B11" s="10"/>
+      <c r="A11" s="13"/>
+      <c r="B11" s="12"/>
       <c r="C11" s="4" t="s">
         <v>98</v>
       </c>
@@ -945,8 +955,8 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
-      <c r="B12" s="10"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="12"/>
       <c r="C12" s="4" t="s">
         <v>104</v>
       </c>
@@ -958,10 +968,10 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="11">
+      <c r="A13" s="13">
         <v>2</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="12" t="s">
         <v>25</v>
       </c>
       <c r="C13" s="4" t="s">
@@ -975,18 +985,19 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="1" t="s">
+      <c r="A14" s="13"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="10" t="s">
         <v>32</v>
       </c>
+      <c r="E14" s="11"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
-      <c r="B15" s="10"/>
+      <c r="A15" s="13"/>
+      <c r="B15" s="12"/>
       <c r="C15" s="4" t="s">
         <v>28</v>
       </c>
@@ -998,8 +1009,8 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
-      <c r="B16" s="10"/>
+      <c r="A16" s="13"/>
+      <c r="B16" s="12"/>
       <c r="C16" s="1" t="s">
         <v>29</v>
       </c>
@@ -1008,8 +1019,8 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
-      <c r="B17" s="10"/>
+      <c r="A17" s="13"/>
+      <c r="B17" s="12"/>
       <c r="C17" s="1" t="s">
         <v>30</v>
       </c>
@@ -1018,10 +1029,10 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="11">
+      <c r="A18" s="13">
         <v>3</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="12" t="s">
         <v>36</v>
       </c>
       <c r="C18" s="4" t="s">
@@ -1035,8 +1046,8 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
-      <c r="B19" s="10"/>
+      <c r="A19" s="13"/>
+      <c r="B19" s="12"/>
       <c r="C19" s="4" t="s">
         <v>38</v>
       </c>
@@ -1048,8 +1059,8 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
-      <c r="B20" s="10"/>
+      <c r="A20" s="13"/>
+      <c r="B20" s="12"/>
       <c r="C20" s="4" t="s">
         <v>39</v>
       </c>
@@ -1061,8 +1072,8 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
-      <c r="B21" s="10"/>
+      <c r="A21" s="13"/>
+      <c r="B21" s="12"/>
       <c r="C21" s="4" t="s">
         <v>40</v>
       </c>
@@ -1074,8 +1085,8 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
-      <c r="B22" s="10"/>
+      <c r="A22" s="13"/>
+      <c r="B22" s="12"/>
       <c r="C22" s="8" t="s">
         <v>102</v>
       </c>
@@ -1085,10 +1096,10 @@
       <c r="E22" s="9"/>
     </row>
     <row r="23" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="11">
+      <c r="A23" s="13">
         <v>4</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="12" t="s">
         <v>45</v>
       </c>
       <c r="C23" s="4" t="s">
@@ -1102,8 +1113,8 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="11"/>
-      <c r="B24" s="10"/>
+      <c r="A24" s="13"/>
+      <c r="B24" s="12"/>
       <c r="C24" s="4" t="s">
         <v>47</v>
       </c>
@@ -1115,8 +1126,8 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="11"/>
-      <c r="B25" s="10"/>
+      <c r="A25" s="13"/>
+      <c r="B25" s="12"/>
       <c r="C25" s="4" t="s">
         <v>48</v>
       </c>
@@ -1128,8 +1139,8 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="11"/>
-      <c r="B26" s="10"/>
+      <c r="A26" s="13"/>
+      <c r="B26" s="12"/>
       <c r="C26" s="4" t="s">
         <v>49</v>
       </c>
@@ -1141,8 +1152,8 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="11"/>
-      <c r="B27" s="10"/>
+      <c r="A27" s="13"/>
+      <c r="B27" s="12"/>
       <c r="C27" s="4" t="s">
         <v>50</v>
       </c>
@@ -1154,8 +1165,8 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="11"/>
-      <c r="B28" s="10"/>
+      <c r="A28" s="13"/>
+      <c r="B28" s="12"/>
       <c r="C28" s="4" t="s">
         <v>51</v>
       </c>
@@ -1167,8 +1178,8 @@
       </c>
     </row>
     <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="11"/>
-      <c r="B29" s="10"/>
+      <c r="A29" s="13"/>
+      <c r="B29" s="12"/>
       <c r="C29" s="8" t="s">
         <v>105</v>
       </c>
@@ -1178,10 +1189,10 @@
       <c r="E29" s="9"/>
     </row>
     <row r="30" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="11">
+      <c r="A30" s="13">
         <v>5</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="12" t="s">
         <v>58</v>
       </c>
       <c r="C30" s="1" t="s">
@@ -1192,8 +1203,8 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="11"/>
-      <c r="B31" s="10"/>
+      <c r="A31" s="13"/>
+      <c r="B31" s="12"/>
       <c r="C31" s="1" t="s">
         <v>60</v>
       </c>
@@ -1202,18 +1213,19 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="11"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="1" t="s">
+      <c r="A32" s="13"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D32" s="8" t="s">
         <v>65</v>
       </c>
+      <c r="E32" s="9"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="11"/>
-      <c r="B33" s="10"/>
+      <c r="A33" s="13"/>
+      <c r="B33" s="12"/>
       <c r="C33" s="1" t="s">
         <v>62</v>
       </c>
@@ -1222,10 +1234,10 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="11">
-        <v>6</v>
-      </c>
-      <c r="B34" s="10" t="s">
+      <c r="A34" s="13">
+        <v>6</v>
+      </c>
+      <c r="B34" s="12" t="s">
         <v>67</v>
       </c>
       <c r="C34" s="1" t="s">
@@ -1236,8 +1248,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="11"/>
-      <c r="B35" s="10"/>
+      <c r="A35" s="13"/>
+      <c r="B35" s="12"/>
       <c r="C35" s="1" t="s">
         <v>69</v>
       </c>
@@ -1246,8 +1258,8 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="11"/>
-      <c r="B36" s="10"/>
+      <c r="A36" s="13"/>
+      <c r="B36" s="12"/>
       <c r="C36" s="1" t="s">
         <v>70</v>
       </c>
@@ -1256,8 +1268,8 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="11"/>
-      <c r="B37" s="10"/>
+      <c r="A37" s="13"/>
+      <c r="B37" s="12"/>
       <c r="C37" s="1" t="s">
         <v>71</v>
       </c>
@@ -1266,10 +1278,10 @@
       </c>
     </row>
     <row r="38" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A38" s="11">
+      <c r="A38" s="13">
         <v>7</v>
       </c>
-      <c r="B38" s="10" t="s">
+      <c r="B38" s="12" t="s">
         <v>76</v>
       </c>
       <c r="C38" s="1" t="s">
@@ -1280,8 +1292,8 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="11"/>
-      <c r="B39" s="10"/>
+      <c r="A39" s="13"/>
+      <c r="B39" s="12"/>
       <c r="C39" s="1" t="s">
         <v>77</v>
       </c>
@@ -1290,8 +1302,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A40" s="11"/>
-      <c r="B40" s="10"/>
+      <c r="A40" s="13"/>
+      <c r="B40" s="12"/>
       <c r="C40" s="1" t="s">
         <v>79</v>
       </c>
@@ -1300,8 +1312,8 @@
       </c>
     </row>
     <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="11"/>
-      <c r="B41" s="10"/>
+      <c r="A41" s="13"/>
+      <c r="B41" s="12"/>
       <c r="C41" s="1" t="s">
         <v>83</v>
       </c>
@@ -1310,10 +1322,10 @@
       </c>
     </row>
     <row r="42" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A42" s="11">
+      <c r="A42" s="13">
         <v>8</v>
       </c>
-      <c r="B42" s="10" t="s">
+      <c r="B42" s="12" t="s">
         <v>85</v>
       </c>
       <c r="C42" s="1" t="s">
@@ -1324,8 +1336,8 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="11"/>
-      <c r="B43" s="10"/>
+      <c r="A43" s="13"/>
+      <c r="B43" s="12"/>
       <c r="C43" s="1" t="s">
         <v>87</v>
       </c>
@@ -1348,10 +1360,10 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A45" s="11">
+      <c r="A45" s="13">
         <v>10</v>
       </c>
-      <c r="B45" s="10" t="s">
+      <c r="B45" s="12" t="s">
         <v>93</v>
       </c>
       <c r="C45" s="1" t="s">
@@ -1362,8 +1374,8 @@
       </c>
     </row>
     <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="11"/>
-      <c r="B46" s="10"/>
+      <c r="A46" s="13"/>
+      <c r="B46" s="12"/>
       <c r="C46" s="1" t="s">
         <v>95</v>
       </c>
@@ -1372,12 +1384,12 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="11"/>
-      <c r="B47" s="10"/>
+      <c r="A47" s="13"/>
+      <c r="B47" s="12"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="11"/>
-      <c r="B48" s="10"/>
+      <c r="A48" s="13"/>
+      <c r="B48" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="18">

</xml_diff>

<commit_message>
NC-2.4 - Integração da rotina de cadastro de usuários com Front-End
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\AppNotificacoesCrimesCidade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67B3763E-80DF-4F50-844E-DEF691198089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EC53B7E-16DC-49A4-8E10-8F9A1FBF7F22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{996D4097-5510-4348-97EC-A204A307EBA8}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="108">
   <si>
     <t>Descrição</t>
   </si>
@@ -384,7 +384,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -403,12 +403,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -422,7 +416,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -445,10 +439,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -792,7 +782,7 @@
   <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="C14:E14"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -821,10 +811,10 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13">
+      <c r="A2" s="11">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="10" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -838,8 +828,8 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="B3" s="12"/>
+      <c r="A3" s="11"/>
+      <c r="B3" s="10"/>
       <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
@@ -851,8 +841,8 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
-      <c r="B4" s="12"/>
+      <c r="A4" s="11"/>
+      <c r="B4" s="10"/>
       <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
@@ -864,8 +854,8 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-      <c r="B5" s="12"/>
+      <c r="A5" s="11"/>
+      <c r="B5" s="10"/>
       <c r="C5" s="4" t="s">
         <v>8</v>
       </c>
@@ -877,8 +867,8 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
-      <c r="B6" s="12"/>
+      <c r="A6" s="11"/>
+      <c r="B6" s="10"/>
       <c r="C6" s="4" t="s">
         <v>9</v>
       </c>
@@ -890,8 +880,8 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
-      <c r="B7" s="12"/>
+      <c r="A7" s="11"/>
+      <c r="B7" s="10"/>
       <c r="C7" s="4" t="s">
         <v>10</v>
       </c>
@@ -903,8 +893,8 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="12"/>
+      <c r="A8" s="11"/>
+      <c r="B8" s="10"/>
       <c r="C8" s="6" t="s">
         <v>11</v>
       </c>
@@ -916,8 +906,8 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="12"/>
+      <c r="A9" s="11"/>
+      <c r="B9" s="10"/>
       <c r="C9" s="4" t="s">
         <v>12</v>
       </c>
@@ -929,8 +919,8 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-      <c r="B10" s="12"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="10"/>
       <c r="C10" s="4" t="s">
         <v>13</v>
       </c>
@@ -942,8 +932,8 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-      <c r="B11" s="12"/>
+      <c r="A11" s="11"/>
+      <c r="B11" s="10"/>
       <c r="C11" s="4" t="s">
         <v>98</v>
       </c>
@@ -955,8 +945,8 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
-      <c r="B12" s="12"/>
+      <c r="A12" s="11"/>
+      <c r="B12" s="10"/>
       <c r="C12" s="4" t="s">
         <v>104</v>
       </c>
@@ -968,10 +958,10 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="13">
+      <c r="A13" s="11">
         <v>2</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="10" t="s">
         <v>25</v>
       </c>
       <c r="C13" s="4" t="s">
@@ -985,19 +975,21 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="10" t="s">
+      <c r="A14" s="11"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="11"/>
+      <c r="E14" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
-      <c r="B15" s="12"/>
+      <c r="A15" s="11"/>
+      <c r="B15" s="10"/>
       <c r="C15" s="4" t="s">
         <v>28</v>
       </c>
@@ -1009,18 +1001,21 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="1" t="s">
+      <c r="A16" s="11"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="4" t="s">
         <v>34</v>
       </c>
+      <c r="E16" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
-      <c r="B17" s="12"/>
+      <c r="A17" s="11"/>
+      <c r="B17" s="10"/>
       <c r="C17" s="1" t="s">
         <v>30</v>
       </c>
@@ -1029,10 +1024,10 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="13">
+      <c r="A18" s="11">
         <v>3</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="10" t="s">
         <v>36</v>
       </c>
       <c r="C18" s="4" t="s">
@@ -1046,8 +1041,8 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
-      <c r="B19" s="12"/>
+      <c r="A19" s="11"/>
+      <c r="B19" s="10"/>
       <c r="C19" s="4" t="s">
         <v>38</v>
       </c>
@@ -1059,8 +1054,8 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
-      <c r="B20" s="12"/>
+      <c r="A20" s="11"/>
+      <c r="B20" s="10"/>
       <c r="C20" s="4" t="s">
         <v>39</v>
       </c>
@@ -1072,8 +1067,8 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
-      <c r="B21" s="12"/>
+      <c r="A21" s="11"/>
+      <c r="B21" s="10"/>
       <c r="C21" s="4" t="s">
         <v>40</v>
       </c>
@@ -1085,8 +1080,8 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="13"/>
-      <c r="B22" s="12"/>
+      <c r="A22" s="11"/>
+      <c r="B22" s="10"/>
       <c r="C22" s="8" t="s">
         <v>102</v>
       </c>
@@ -1096,10 +1091,10 @@
       <c r="E22" s="9"/>
     </row>
     <row r="23" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="13">
+      <c r="A23" s="11">
         <v>4</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="10" t="s">
         <v>45</v>
       </c>
       <c r="C23" s="4" t="s">
@@ -1113,8 +1108,8 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="13"/>
-      <c r="B24" s="12"/>
+      <c r="A24" s="11"/>
+      <c r="B24" s="10"/>
       <c r="C24" s="4" t="s">
         <v>47</v>
       </c>
@@ -1126,8 +1121,8 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="13"/>
-      <c r="B25" s="12"/>
+      <c r="A25" s="11"/>
+      <c r="B25" s="10"/>
       <c r="C25" s="4" t="s">
         <v>48</v>
       </c>
@@ -1139,8 +1134,8 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="13"/>
-      <c r="B26" s="12"/>
+      <c r="A26" s="11"/>
+      <c r="B26" s="10"/>
       <c r="C26" s="4" t="s">
         <v>49</v>
       </c>
@@ -1152,8 +1147,8 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="13"/>
-      <c r="B27" s="12"/>
+      <c r="A27" s="11"/>
+      <c r="B27" s="10"/>
       <c r="C27" s="4" t="s">
         <v>50</v>
       </c>
@@ -1165,8 +1160,8 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="13"/>
-      <c r="B28" s="12"/>
+      <c r="A28" s="11"/>
+      <c r="B28" s="10"/>
       <c r="C28" s="4" t="s">
         <v>51</v>
       </c>
@@ -1178,8 +1173,8 @@
       </c>
     </row>
     <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="13"/>
-      <c r="B29" s="12"/>
+      <c r="A29" s="11"/>
+      <c r="B29" s="10"/>
       <c r="C29" s="8" t="s">
         <v>105</v>
       </c>
@@ -1189,10 +1184,10 @@
       <c r="E29" s="9"/>
     </row>
     <row r="30" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="13">
+      <c r="A30" s="11">
         <v>5</v>
       </c>
-      <c r="B30" s="12" t="s">
+      <c r="B30" s="10" t="s">
         <v>58</v>
       </c>
       <c r="C30" s="1" t="s">
@@ -1203,8 +1198,8 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="13"/>
-      <c r="B31" s="12"/>
+      <c r="A31" s="11"/>
+      <c r="B31" s="10"/>
       <c r="C31" s="1" t="s">
         <v>60</v>
       </c>
@@ -1213,8 +1208,8 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="13"/>
-      <c r="B32" s="12"/>
+      <c r="A32" s="11"/>
+      <c r="B32" s="10"/>
       <c r="C32" s="8" t="s">
         <v>61</v>
       </c>
@@ -1224,8 +1219,8 @@
       <c r="E32" s="9"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="13"/>
-      <c r="B33" s="12"/>
+      <c r="A33" s="11"/>
+      <c r="B33" s="10"/>
       <c r="C33" s="1" t="s">
         <v>62</v>
       </c>
@@ -1234,10 +1229,10 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="13">
-        <v>6</v>
-      </c>
-      <c r="B34" s="12" t="s">
+      <c r="A34" s="11">
+        <v>6</v>
+      </c>
+      <c r="B34" s="10" t="s">
         <v>67</v>
       </c>
       <c r="C34" s="1" t="s">
@@ -1248,8 +1243,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="13"/>
-      <c r="B35" s="12"/>
+      <c r="A35" s="11"/>
+      <c r="B35" s="10"/>
       <c r="C35" s="1" t="s">
         <v>69</v>
       </c>
@@ -1258,8 +1253,8 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="13"/>
-      <c r="B36" s="12"/>
+      <c r="A36" s="11"/>
+      <c r="B36" s="10"/>
       <c r="C36" s="1" t="s">
         <v>70</v>
       </c>
@@ -1268,8 +1263,8 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="13"/>
-      <c r="B37" s="12"/>
+      <c r="A37" s="11"/>
+      <c r="B37" s="10"/>
       <c r="C37" s="1" t="s">
         <v>71</v>
       </c>
@@ -1278,10 +1273,10 @@
       </c>
     </row>
     <row r="38" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A38" s="13">
+      <c r="A38" s="11">
         <v>7</v>
       </c>
-      <c r="B38" s="12" t="s">
+      <c r="B38" s="10" t="s">
         <v>76</v>
       </c>
       <c r="C38" s="1" t="s">
@@ -1292,8 +1287,8 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="13"/>
-      <c r="B39" s="12"/>
+      <c r="A39" s="11"/>
+      <c r="B39" s="10"/>
       <c r="C39" s="1" t="s">
         <v>77</v>
       </c>
@@ -1302,8 +1297,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A40" s="13"/>
-      <c r="B40" s="12"/>
+      <c r="A40" s="11"/>
+      <c r="B40" s="10"/>
       <c r="C40" s="1" t="s">
         <v>79</v>
       </c>
@@ -1312,8 +1307,8 @@
       </c>
     </row>
     <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="13"/>
-      <c r="B41" s="12"/>
+      <c r="A41" s="11"/>
+      <c r="B41" s="10"/>
       <c r="C41" s="1" t="s">
         <v>83</v>
       </c>
@@ -1322,10 +1317,10 @@
       </c>
     </row>
     <row r="42" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A42" s="13">
+      <c r="A42" s="11">
         <v>8</v>
       </c>
-      <c r="B42" s="12" t="s">
+      <c r="B42" s="10" t="s">
         <v>85</v>
       </c>
       <c r="C42" s="1" t="s">
@@ -1336,8 +1331,8 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="13"/>
-      <c r="B43" s="12"/>
+      <c r="A43" s="11"/>
+      <c r="B43" s="10"/>
       <c r="C43" s="1" t="s">
         <v>87</v>
       </c>
@@ -1360,10 +1355,10 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A45" s="13">
+      <c r="A45" s="11">
         <v>10</v>
       </c>
-      <c r="B45" s="12" t="s">
+      <c r="B45" s="10" t="s">
         <v>93</v>
       </c>
       <c r="C45" s="1" t="s">
@@ -1374,8 +1369,8 @@
       </c>
     </row>
     <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="13"/>
-      <c r="B46" s="12"/>
+      <c r="A46" s="11"/>
+      <c r="B46" s="10"/>
       <c r="C46" s="1" t="s">
         <v>95</v>
       </c>
@@ -1384,12 +1379,12 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="13"/>
-      <c r="B47" s="12"/>
+      <c r="A47" s="11"/>
+      <c r="B47" s="10"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="13"/>
-      <c r="B48" s="12"/>
+      <c r="A48" s="11"/>
+      <c r="B48" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="18">

</xml_diff>

<commit_message>
NC-7.2 - Notificações através do firebase cloud message
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\AppNotificacoesCrimesCidade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EC53B7E-16DC-49A4-8E10-8F9A1FBF7F22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{609C3E22-2041-4784-A387-C3EDA2C851FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{996D4097-5510-4348-97EC-A204A307EBA8}"/>
   </bookViews>
@@ -384,7 +384,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -403,6 +403,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -416,7 +422,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -444,6 +450,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -781,8 +790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94151779-DED3-44C5-B19B-FEA501E890E9}">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1289,10 +1298,10 @@
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="11"/>
       <c r="B39" s="10"/>
-      <c r="C39" s="1" t="s">
+      <c r="C39" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D39" s="12" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1388,24 +1397,24 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B13:B17"/>
+    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="A18:A22"/>
+    <mergeCell ref="B18:B22"/>
+    <mergeCell ref="A2:A12"/>
+    <mergeCell ref="B2:B12"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="B23:B29"/>
+    <mergeCell ref="A23:A29"/>
     <mergeCell ref="B45:B48"/>
     <mergeCell ref="A45:A48"/>
     <mergeCell ref="B38:B41"/>
     <mergeCell ref="A38:A41"/>
     <mergeCell ref="B42:B43"/>
     <mergeCell ref="A42:A43"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="B23:B29"/>
-    <mergeCell ref="A23:A29"/>
-    <mergeCell ref="B13:B17"/>
-    <mergeCell ref="A13:A17"/>
-    <mergeCell ref="A18:A22"/>
-    <mergeCell ref="B18:B22"/>
-    <mergeCell ref="A2:A12"/>
-    <mergeCell ref="B2:B12"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
NC-7.3 - Integração das notificações com o cadastro de ocorrências e os locais do usuário
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\AppNotificacoesCrimesCidade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{609C3E22-2041-4784-A387-C3EDA2C851FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B29465A-6EB5-4372-BA9D-56508F4A73B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{996D4097-5510-4348-97EC-A204A307EBA8}"/>
+    <workbookView xWindow="-19320" yWindow="780" windowWidth="19440" windowHeight="10440" xr2:uid="{996D4097-5510-4348-97EC-A204A307EBA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="108">
   <si>
     <t>Descrição</t>
   </si>
@@ -422,7 +422,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -445,14 +445,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -790,8 +791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94151779-DED3-44C5-B19B-FEA501E890E9}">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,10 +821,10 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11">
+      <c r="A2" s="13">
         <v>1</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="12" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -837,8 +838,8 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="10"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="12"/>
       <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
@@ -850,8 +851,8 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="10"/>
+      <c r="A4" s="13"/>
+      <c r="B4" s="12"/>
       <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
@@ -863,8 +864,8 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="10"/>
+      <c r="A5" s="13"/>
+      <c r="B5" s="12"/>
       <c r="C5" s="4" t="s">
         <v>8</v>
       </c>
@@ -876,8 +877,8 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="10"/>
+      <c r="A6" s="13"/>
+      <c r="B6" s="12"/>
       <c r="C6" s="4" t="s">
         <v>9</v>
       </c>
@@ -889,8 +890,8 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="10"/>
+      <c r="A7" s="13"/>
+      <c r="B7" s="12"/>
       <c r="C7" s="4" t="s">
         <v>10</v>
       </c>
@@ -902,8 +903,8 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
-      <c r="B8" s="10"/>
+      <c r="A8" s="13"/>
+      <c r="B8" s="12"/>
       <c r="C8" s="6" t="s">
         <v>11</v>
       </c>
@@ -915,8 +916,8 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
-      <c r="B9" s="10"/>
+      <c r="A9" s="13"/>
+      <c r="B9" s="12"/>
       <c r="C9" s="4" t="s">
         <v>12</v>
       </c>
@@ -928,8 +929,8 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
-      <c r="B10" s="10"/>
+      <c r="A10" s="13"/>
+      <c r="B10" s="12"/>
       <c r="C10" s="4" t="s">
         <v>13</v>
       </c>
@@ -941,8 +942,8 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
-      <c r="B11" s="10"/>
+      <c r="A11" s="13"/>
+      <c r="B11" s="12"/>
       <c r="C11" s="4" t="s">
         <v>98</v>
       </c>
@@ -954,8 +955,8 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
-      <c r="B12" s="10"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="12"/>
       <c r="C12" s="4" t="s">
         <v>104</v>
       </c>
@@ -967,10 +968,10 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="11">
+      <c r="A13" s="13">
         <v>2</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="12" t="s">
         <v>25</v>
       </c>
       <c r="C13" s="4" t="s">
@@ -984,8 +985,8 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
-      <c r="B14" s="10"/>
+      <c r="A14" s="13"/>
+      <c r="B14" s="12"/>
       <c r="C14" s="4" t="s">
         <v>27</v>
       </c>
@@ -997,8 +998,8 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
-      <c r="B15" s="10"/>
+      <c r="A15" s="13"/>
+      <c r="B15" s="12"/>
       <c r="C15" s="4" t="s">
         <v>28</v>
       </c>
@@ -1010,8 +1011,8 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
-      <c r="B16" s="10"/>
+      <c r="A16" s="13"/>
+      <c r="B16" s="12"/>
       <c r="C16" s="4" t="s">
         <v>29</v>
       </c>
@@ -1023,8 +1024,8 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
-      <c r="B17" s="10"/>
+      <c r="A17" s="13"/>
+      <c r="B17" s="12"/>
       <c r="C17" s="1" t="s">
         <v>30</v>
       </c>
@@ -1033,10 +1034,10 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="11">
+      <c r="A18" s="13">
         <v>3</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="12" t="s">
         <v>36</v>
       </c>
       <c r="C18" s="4" t="s">
@@ -1050,8 +1051,8 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
-      <c r="B19" s="10"/>
+      <c r="A19" s="13"/>
+      <c r="B19" s="12"/>
       <c r="C19" s="4" t="s">
         <v>38</v>
       </c>
@@ -1063,8 +1064,8 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
-      <c r="B20" s="10"/>
+      <c r="A20" s="13"/>
+      <c r="B20" s="12"/>
       <c r="C20" s="4" t="s">
         <v>39</v>
       </c>
@@ -1076,8 +1077,8 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
-      <c r="B21" s="10"/>
+      <c r="A21" s="13"/>
+      <c r="B21" s="12"/>
       <c r="C21" s="4" t="s">
         <v>40</v>
       </c>
@@ -1089,8 +1090,8 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
-      <c r="B22" s="10"/>
+      <c r="A22" s="13"/>
+      <c r="B22" s="12"/>
       <c r="C22" s="8" t="s">
         <v>102</v>
       </c>
@@ -1100,10 +1101,10 @@
       <c r="E22" s="9"/>
     </row>
     <row r="23" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="11">
+      <c r="A23" s="13">
         <v>4</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="12" t="s">
         <v>45</v>
       </c>
       <c r="C23" s="4" t="s">
@@ -1117,8 +1118,8 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="11"/>
-      <c r="B24" s="10"/>
+      <c r="A24" s="13"/>
+      <c r="B24" s="12"/>
       <c r="C24" s="4" t="s">
         <v>47</v>
       </c>
@@ -1130,8 +1131,8 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="11"/>
-      <c r="B25" s="10"/>
+      <c r="A25" s="13"/>
+      <c r="B25" s="12"/>
       <c r="C25" s="4" t="s">
         <v>48</v>
       </c>
@@ -1143,8 +1144,8 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="11"/>
-      <c r="B26" s="10"/>
+      <c r="A26" s="13"/>
+      <c r="B26" s="12"/>
       <c r="C26" s="4" t="s">
         <v>49</v>
       </c>
@@ -1156,8 +1157,8 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="11"/>
-      <c r="B27" s="10"/>
+      <c r="A27" s="13"/>
+      <c r="B27" s="12"/>
       <c r="C27" s="4" t="s">
         <v>50</v>
       </c>
@@ -1169,8 +1170,8 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="11"/>
-      <c r="B28" s="10"/>
+      <c r="A28" s="13"/>
+      <c r="B28" s="12"/>
       <c r="C28" s="4" t="s">
         <v>51</v>
       </c>
@@ -1182,8 +1183,8 @@
       </c>
     </row>
     <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="11"/>
-      <c r="B29" s="10"/>
+      <c r="A29" s="13"/>
+      <c r="B29" s="12"/>
       <c r="C29" s="8" t="s">
         <v>105</v>
       </c>
@@ -1193,10 +1194,10 @@
       <c r="E29" s="9"/>
     </row>
     <row r="30" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="11">
+      <c r="A30" s="13">
         <v>5</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="12" t="s">
         <v>58</v>
       </c>
       <c r="C30" s="1" t="s">
@@ -1207,8 +1208,8 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="11"/>
-      <c r="B31" s="10"/>
+      <c r="A31" s="13"/>
+      <c r="B31" s="12"/>
       <c r="C31" s="1" t="s">
         <v>60</v>
       </c>
@@ -1217,8 +1218,8 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="11"/>
-      <c r="B32" s="10"/>
+      <c r="A32" s="13"/>
+      <c r="B32" s="12"/>
       <c r="C32" s="8" t="s">
         <v>61</v>
       </c>
@@ -1227,9 +1228,9 @@
       </c>
       <c r="E32" s="9"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="11"/>
-      <c r="B33" s="10"/>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="13"/>
+      <c r="B33" s="12"/>
       <c r="C33" s="1" t="s">
         <v>62</v>
       </c>
@@ -1237,11 +1238,11 @@
         <v>66</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="11">
-        <v>6</v>
-      </c>
-      <c r="B34" s="10" t="s">
+    <row r="34" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="13">
+        <v>6</v>
+      </c>
+      <c r="B34" s="12" t="s">
         <v>67</v>
       </c>
       <c r="C34" s="1" t="s">
@@ -1251,9 +1252,9 @@
         <v>72</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="11"/>
-      <c r="B35" s="10"/>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="13"/>
+      <c r="B35" s="12"/>
       <c r="C35" s="1" t="s">
         <v>69</v>
       </c>
@@ -1261,9 +1262,9 @@
         <v>73</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="11"/>
-      <c r="B36" s="10"/>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="13"/>
+      <c r="B36" s="12"/>
       <c r="C36" s="1" t="s">
         <v>70</v>
       </c>
@@ -1271,9 +1272,9 @@
         <v>74</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="11"/>
-      <c r="B37" s="10"/>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="13"/>
+      <c r="B37" s="12"/>
       <c r="C37" s="1" t="s">
         <v>71</v>
       </c>
@@ -1281,11 +1282,11 @@
         <v>75</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A38" s="11">
+    <row r="38" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A38" s="13">
         <v>7</v>
       </c>
-      <c r="B38" s="10" t="s">
+      <c r="B38" s="12" t="s">
         <v>76</v>
       </c>
       <c r="C38" s="1" t="s">
@@ -1295,29 +1296,33 @@
         <v>80</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="11"/>
-      <c r="B39" s="10"/>
-      <c r="C39" s="12" t="s">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="13"/>
+      <c r="B39" s="12"/>
+      <c r="C39" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="D39" s="12" t="s">
+      <c r="D39" s="4" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A40" s="11"/>
-      <c r="B40" s="10"/>
-      <c r="C40" s="1" t="s">
+      <c r="E39" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A40" s="13"/>
+      <c r="B40" s="12"/>
+      <c r="C40" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="D40" s="10" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="11"/>
-      <c r="B41" s="10"/>
+      <c r="E40" s="11"/>
+    </row>
+    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="13"/>
+      <c r="B41" s="12"/>
       <c r="C41" s="1" t="s">
         <v>83</v>
       </c>
@@ -1325,11 +1330,11 @@
         <v>84</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A42" s="11">
+    <row r="42" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A42" s="13">
         <v>8</v>
       </c>
-      <c r="B42" s="10" t="s">
+      <c r="B42" s="12" t="s">
         <v>85</v>
       </c>
       <c r="C42" s="1" t="s">
@@ -1339,9 +1344,9 @@
         <v>88</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="11"/>
-      <c r="B43" s="10"/>
+    <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="13"/>
+      <c r="B43" s="12"/>
       <c r="C43" s="1" t="s">
         <v>87</v>
       </c>
@@ -1349,7 +1354,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>9</v>
       </c>
@@ -1363,11 +1368,11 @@
         <v>92</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A45" s="11">
+    <row r="45" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A45" s="13">
         <v>10</v>
       </c>
-      <c r="B45" s="10" t="s">
+      <c r="B45" s="12" t="s">
         <v>93</v>
       </c>
       <c r="C45" s="1" t="s">
@@ -1377,9 +1382,9 @@
         <v>96</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="11"/>
-      <c r="B46" s="10"/>
+    <row r="46" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="13"/>
+      <c r="B46" s="12"/>
       <c r="C46" s="1" t="s">
         <v>95</v>
       </c>
@@ -1387,13 +1392,13 @@
         <v>97</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="11"/>
-      <c r="B47" s="10"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="11"/>
-      <c r="B48" s="10"/>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="13"/>
+      <c r="B47" s="12"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="13"/>
+      <c r="B48" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="18">

</xml_diff>

<commit_message>
NC - 6.1, 6.2, 6.3 - Implementado as rotinas para visualização e edição das configurações
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\AppNotificacoesCrimesCidade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B29465A-6EB5-4372-BA9D-56508F4A73B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE2F3FD7-6E68-49F6-8F40-C0BCF29A21D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="780" windowWidth="19440" windowHeight="10440" xr2:uid="{996D4097-5510-4348-97EC-A204A307EBA8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{996D4097-5510-4348-97EC-A204A307EBA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="108">
   <si>
     <t>Descrição</t>
   </si>
@@ -422,7 +422,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -454,6 +454,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -791,8 +797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94151779-DED3-44C5-B19B-FEA501E890E9}">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1194,49 +1200,52 @@
       <c r="E29" s="9"/>
     </row>
     <row r="30" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="13">
+      <c r="A30" s="14">
         <v>5</v>
       </c>
-      <c r="B30" s="12" t="s">
+      <c r="B30" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D30" s="4" t="s">
         <v>63</v>
       </c>
+      <c r="E30" s="5"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="13"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="1" t="s">
+      <c r="A31" s="14"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D31" s="4" t="s">
         <v>64</v>
       </c>
+      <c r="E31" s="5"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="13"/>
-      <c r="B32" s="12"/>
-      <c r="C32" s="8" t="s">
+      <c r="A32" s="14"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="D32" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="E32" s="9"/>
+      <c r="E32" s="5"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="13"/>
-      <c r="B33" s="12"/>
-      <c r="C33" s="1" t="s">
+      <c r="A33" s="14"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D33" s="4" t="s">
         <v>66</v>
       </c>
+      <c r="E33" s="5"/>
     </row>
     <row r="34" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="13">
@@ -1255,12 +1264,13 @@
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="13"/>
       <c r="B35" s="12"/>
-      <c r="C35" s="1" t="s">
+      <c r="C35" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D35" s="10" t="s">
         <v>73</v>
       </c>
+      <c r="E35" s="11"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="13"/>
@@ -1312,13 +1322,15 @@
     <row r="40" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="13"/>
       <c r="B40" s="12"/>
-      <c r="C40" s="10" t="s">
+      <c r="C40" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D40" s="10" t="s">
+      <c r="D40" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="E40" s="11"/>
+      <c r="E40" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="13"/>
@@ -1402,24 +1414,24 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="B23:B29"/>
+    <mergeCell ref="A23:A29"/>
     <mergeCell ref="B13:B17"/>
     <mergeCell ref="A13:A17"/>
     <mergeCell ref="A18:A22"/>
     <mergeCell ref="B18:B22"/>
     <mergeCell ref="A2:A12"/>
     <mergeCell ref="B2:B12"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="B23:B29"/>
-    <mergeCell ref="A23:A29"/>
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="B38:B41"/>
-    <mergeCell ref="A38:A41"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="A42:A43"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
NC-7.5 - Implementado rotina para buscar localização do usuário
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\AppNotificacoesCrimesCidade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{548DA1A1-CBEE-4C91-8E51-34AC54EE4BCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D02241-83BA-4B9D-8B1D-F098B709FC99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="-1545" windowWidth="21840" windowHeight="13140" xr2:uid="{996D4097-5510-4348-97EC-A204A307EBA8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{996D4097-5510-4348-97EC-A204A307EBA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -434,10 +434,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -782,7 +782,7 @@
   <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="D43" sqref="C43:D43"/>
+      <selection activeCell="D44" sqref="C44:D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -807,10 +807,10 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
+      <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -821,8 +821,8 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="7"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="6"/>
       <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
@@ -831,8 +831,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="7"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="6"/>
       <c r="C4" s="4" t="s">
         <v>5</v>
       </c>
@@ -841,8 +841,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="7"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="6"/>
       <c r="C5" s="4" t="s">
         <v>6</v>
       </c>
@@ -851,8 +851,8 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="7"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="6"/>
       <c r="C6" s="4" t="s">
         <v>7</v>
       </c>
@@ -861,8 +861,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="7"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="6"/>
       <c r="C7" s="4" t="s">
         <v>8</v>
       </c>
@@ -871,8 +871,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="7"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="6"/>
       <c r="C8" s="4" t="s">
         <v>9</v>
       </c>
@@ -881,8 +881,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="7"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="6"/>
       <c r="C9" s="4" t="s">
         <v>10</v>
       </c>
@@ -891,8 +891,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="7"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="6"/>
       <c r="C10" s="4" t="s">
         <v>11</v>
       </c>
@@ -901,8 +901,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="7"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="6"/>
       <c r="C11" s="4" t="s">
         <v>96</v>
       </c>
@@ -911,8 +911,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="7"/>
+      <c r="A12" s="7"/>
+      <c r="B12" s="6"/>
       <c r="C12" s="4" t="s">
         <v>101</v>
       </c>
@@ -921,8 +921,8 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="7"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="6"/>
       <c r="C13" s="5" t="s">
         <v>104</v>
       </c>
@@ -931,10 +931,10 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
+      <c r="A14" s="7">
         <v>2</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -945,8 +945,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="7"/>
+      <c r="A15" s="7"/>
+      <c r="B15" s="6"/>
       <c r="C15" s="4" t="s">
         <v>25</v>
       </c>
@@ -955,8 +955,8 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="7"/>
+      <c r="A16" s="7"/>
+      <c r="B16" s="6"/>
       <c r="C16" s="4" t="s">
         <v>26</v>
       </c>
@@ -965,8 +965,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="B17" s="7"/>
+      <c r="A17" s="7"/>
+      <c r="B17" s="6"/>
       <c r="C17" s="4" t="s">
         <v>27</v>
       </c>
@@ -975,8 +975,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="7"/>
+      <c r="A18" s="7"/>
+      <c r="B18" s="6"/>
       <c r="C18" s="1" t="s">
         <v>28</v>
       </c>
@@ -985,8 +985,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="7"/>
+      <c r="A19" s="7"/>
+      <c r="B19" s="6"/>
       <c r="C19" s="1" t="s">
         <v>106</v>
       </c>
@@ -995,10 +995,10 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="6">
+      <c r="A20" s="7">
         <v>3</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C20" s="4" t="s">
@@ -1009,8 +1009,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
-      <c r="B21" s="7"/>
+      <c r="A21" s="7"/>
+      <c r="B21" s="6"/>
       <c r="C21" s="4" t="s">
         <v>36</v>
       </c>
@@ -1019,8 +1019,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="7"/>
+      <c r="A22" s="7"/>
+      <c r="B22" s="6"/>
       <c r="C22" s="4" t="s">
         <v>37</v>
       </c>
@@ -1029,8 +1029,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-      <c r="B23" s="7"/>
+      <c r="A23" s="7"/>
+      <c r="B23" s="6"/>
       <c r="C23" s="4" t="s">
         <v>38</v>
       </c>
@@ -1039,8 +1039,8 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="B24" s="7"/>
+      <c r="A24" s="7"/>
+      <c r="B24" s="6"/>
       <c r="C24" s="5" t="s">
         <v>99</v>
       </c>
@@ -1049,10 +1049,10 @@
       </c>
     </row>
     <row r="25" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="6">
+      <c r="A25" s="7">
         <v>4</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="6" t="s">
         <v>43</v>
       </c>
       <c r="C25" s="4" t="s">
@@ -1063,8 +1063,8 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
-      <c r="B26" s="7"/>
+      <c r="A26" s="7"/>
+      <c r="B26" s="6"/>
       <c r="C26" s="4" t="s">
         <v>45</v>
       </c>
@@ -1073,8 +1073,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-      <c r="B27" s="7"/>
+      <c r="A27" s="7"/>
+      <c r="B27" s="6"/>
       <c r="C27" s="4" t="s">
         <v>46</v>
       </c>
@@ -1083,8 +1083,8 @@
       </c>
     </row>
     <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-      <c r="B28" s="7"/>
+      <c r="A28" s="7"/>
+      <c r="B28" s="6"/>
       <c r="C28" s="4" t="s">
         <v>47</v>
       </c>
@@ -1093,8 +1093,8 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
-      <c r="B29" s="7"/>
+      <c r="A29" s="7"/>
+      <c r="B29" s="6"/>
       <c r="C29" s="4" t="s">
         <v>48</v>
       </c>
@@ -1103,8 +1103,8 @@
       </c>
     </row>
     <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="6"/>
-      <c r="B30" s="7"/>
+      <c r="A30" s="7"/>
+      <c r="B30" s="6"/>
       <c r="C30" s="4" t="s">
         <v>49</v>
       </c>
@@ -1113,8 +1113,8 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="6"/>
-      <c r="B31" s="7"/>
+      <c r="A31" s="7"/>
+      <c r="B31" s="6"/>
       <c r="C31" s="5" t="s">
         <v>102</v>
       </c>
@@ -1167,10 +1167,10 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="6">
+      <c r="A36" s="7">
         <v>6</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="B36" s="6" t="s">
         <v>65</v>
       </c>
       <c r="C36" s="4" t="s">
@@ -1181,8 +1181,8 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="6"/>
-      <c r="B37" s="7"/>
+      <c r="A37" s="7"/>
+      <c r="B37" s="6"/>
       <c r="C37" s="4" t="s">
         <v>67</v>
       </c>
@@ -1191,8 +1191,8 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="6"/>
-      <c r="B38" s="7"/>
+      <c r="A38" s="7"/>
+      <c r="B38" s="6"/>
       <c r="C38" s="4" t="s">
         <v>68</v>
       </c>
@@ -1201,8 +1201,8 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="6"/>
-      <c r="B39" s="7"/>
+      <c r="A39" s="7"/>
+      <c r="B39" s="6"/>
       <c r="C39" s="1" t="s">
         <v>69</v>
       </c>
@@ -1211,10 +1211,10 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A40" s="6">
+      <c r="A40" s="7">
         <v>7</v>
       </c>
-      <c r="B40" s="7" t="s">
+      <c r="B40" s="6" t="s">
         <v>74</v>
       </c>
       <c r="C40" s="1" t="s">
@@ -1225,8 +1225,8 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="6"/>
-      <c r="B41" s="7"/>
+      <c r="A41" s="7"/>
+      <c r="B41" s="6"/>
       <c r="C41" s="4" t="s">
         <v>75</v>
       </c>
@@ -1235,8 +1235,8 @@
       </c>
     </row>
     <row r="42" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A42" s="6"/>
-      <c r="B42" s="7"/>
+      <c r="A42" s="7"/>
+      <c r="B42" s="6"/>
       <c r="C42" s="4" t="s">
         <v>77</v>
       </c>
@@ -1245,8 +1245,8 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="6"/>
-      <c r="B43" s="7"/>
+      <c r="A43" s="7"/>
+      <c r="B43" s="6"/>
       <c r="C43" s="4" t="s">
         <v>81</v>
       </c>
@@ -1255,20 +1255,20 @@
       </c>
     </row>
     <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="6"/>
-      <c r="B44" s="7"/>
-      <c r="C44" s="1" t="s">
+      <c r="A44" s="7"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="D44" s="4" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A45" s="6">
+      <c r="A45" s="7">
         <v>8</v>
       </c>
-      <c r="B45" s="7" t="s">
+      <c r="B45" s="6" t="s">
         <v>83</v>
       </c>
       <c r="C45" s="1" t="s">
@@ -1279,8 +1279,8 @@
       </c>
     </row>
     <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="6"/>
-      <c r="B46" s="7"/>
+      <c r="A46" s="7"/>
+      <c r="B46" s="6"/>
       <c r="C46" s="1" t="s">
         <v>85</v>
       </c>
@@ -1303,10 +1303,10 @@
       </c>
     </row>
     <row r="48" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A48" s="6">
+      <c r="A48" s="7">
         <v>10</v>
       </c>
-      <c r="B48" s="7" t="s">
+      <c r="B48" s="6" t="s">
         <v>91</v>
       </c>
       <c r="C48" s="1" t="s">
@@ -1317,8 +1317,8 @@
       </c>
     </row>
     <row r="49" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" s="6"/>
-      <c r="B49" s="7"/>
+      <c r="A49" s="7"/>
+      <c r="B49" s="6"/>
       <c r="C49" s="1" t="s">
         <v>93</v>
       </c>
@@ -1327,33 +1327,33 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="6"/>
-      <c r="B50" s="7"/>
+      <c r="A50" s="7"/>
+      <c r="B50" s="6"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="6"/>
-      <c r="B51" s="7"/>
+      <c r="A51" s="7"/>
+      <c r="B51" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A20:A24"/>
+    <mergeCell ref="B20:B24"/>
+    <mergeCell ref="B2:B13"/>
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="B14:B19"/>
+    <mergeCell ref="A14:A19"/>
+    <mergeCell ref="B32:B35"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="B36:B39"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="B25:B31"/>
+    <mergeCell ref="A25:A31"/>
     <mergeCell ref="B48:B51"/>
     <mergeCell ref="A48:A51"/>
     <mergeCell ref="B45:B46"/>
     <mergeCell ref="A45:A46"/>
     <mergeCell ref="B40:B44"/>
     <mergeCell ref="A40:A44"/>
-    <mergeCell ref="B32:B35"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="B36:B39"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="B25:B31"/>
-    <mergeCell ref="A25:A31"/>
-    <mergeCell ref="A20:A24"/>
-    <mergeCell ref="B20:B24"/>
-    <mergeCell ref="B2:B13"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="B14:B19"/>
-    <mergeCell ref="A14:A19"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
NC-2.6 - Validação de email único + remoção de alterações que devem ficar para próxima versão
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\AppNotificacoesCrimesCidade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D02241-83BA-4B9D-8B1D-F098B709FC99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F15F4D40-F897-4647-B623-F1301235B13D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{996D4097-5510-4348-97EC-A204A307EBA8}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="113">
   <si>
     <t>Descrição</t>
   </si>
@@ -369,6 +369,15 @@
   </si>
   <si>
     <t>7.5</t>
+  </si>
+  <si>
+    <t>Próxima versão</t>
+  </si>
+  <si>
+    <t>Rotina de validação de email</t>
+  </si>
+  <si>
+    <t>2.7</t>
   </si>
 </sst>
 </file>
@@ -390,7 +399,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -400,6 +409,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -416,7 +431,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -434,16 +449,31 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -779,10 +809,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94151779-DED3-44C5-B19B-FEA501E890E9}">
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="D44" sqref="C44:D44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="C19:D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -790,6 +820,7 @@
     <col min="1" max="1" width="9.140625" style="2"/>
     <col min="2" max="2" width="39.28515625" style="3" customWidth="1"/>
     <col min="3" max="4" width="52.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -807,10 +838,10 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -821,8 +852,8 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="6"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="7"/>
       <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
@@ -831,8 +862,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="6"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="7"/>
       <c r="C4" s="4" t="s">
         <v>5</v>
       </c>
@@ -841,8 +872,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="6"/>
+      <c r="A5" s="6"/>
+      <c r="B5" s="7"/>
       <c r="C5" s="4" t="s">
         <v>6</v>
       </c>
@@ -851,8 +882,8 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="6"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="7"/>
       <c r="C6" s="4" t="s">
         <v>7</v>
       </c>
@@ -861,8 +892,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="6"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="7"/>
       <c r="C7" s="4" t="s">
         <v>8</v>
       </c>
@@ -871,8 +902,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="6"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="7"/>
       <c r="C8" s="4" t="s">
         <v>9</v>
       </c>
@@ -881,8 +912,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="6"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="7"/>
       <c r="C9" s="4" t="s">
         <v>10</v>
       </c>
@@ -891,8 +922,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="B10" s="6"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="7"/>
       <c r="C10" s="4" t="s">
         <v>11</v>
       </c>
@@ -901,8 +932,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="6"/>
+      <c r="A11" s="6"/>
+      <c r="B11" s="7"/>
       <c r="C11" s="4" t="s">
         <v>96</v>
       </c>
@@ -911,8 +942,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="6"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="7"/>
       <c r="C12" s="4" t="s">
         <v>101</v>
       </c>
@@ -921,8 +952,8 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="6"/>
+      <c r="A13" s="6"/>
+      <c r="B13" s="7"/>
       <c r="C13" s="5" t="s">
         <v>104</v>
       </c>
@@ -931,10 +962,10 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="7">
+      <c r="A14" s="6">
         <v>2</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="7" t="s">
         <v>23</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -945,8 +976,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="6"/>
+      <c r="A15" s="6"/>
+      <c r="B15" s="7"/>
       <c r="C15" s="4" t="s">
         <v>25</v>
       </c>
@@ -955,8 +986,8 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
-      <c r="B16" s="6"/>
+      <c r="A16" s="6"/>
+      <c r="B16" s="7"/>
       <c r="C16" s="4" t="s">
         <v>26</v>
       </c>
@@ -964,9 +995,9 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
-      <c r="B17" s="6"/>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="6"/>
+      <c r="B17" s="7"/>
       <c r="C17" s="4" t="s">
         <v>27</v>
       </c>
@@ -974,386 +1005,430 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="1" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="6"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="10" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="1" t="s">
+      <c r="E18" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="4" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="7">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="6">
         <v>3</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B21" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C21" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D21" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="4" t="s">
+    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="6"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D22" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="4" t="s">
+    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D23" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="4" t="s">
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="6"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D24" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="5" t="s">
+    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="6"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D25" s="5" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="7">
+    <row r="26" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="6">
         <v>4</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B26" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C26" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D26" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="4" t="s">
+    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="6"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D27" s="4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="4" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="6"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D28" s="4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="4" t="s">
+    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="6"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D29" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="4" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="6"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D30" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="7"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="4" t="s">
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="6"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D31" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="5" t="s">
+    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="6"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D32" s="10" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="9">
+      <c r="E32" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="9">
         <v>5</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B33" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C33" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D33" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="9"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="9"/>
       <c r="B34" s="8"/>
       <c r="C34" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="9"/>
       <c r="B35" s="8"/>
       <c r="C35" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="9"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="D36" s="4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="7">
+    <row r="37" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="6">
         <v>6</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B37" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C37" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="D37" s="4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="7"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="4" t="s">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="6"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="D38" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="7"/>
-      <c r="B38" s="6"/>
-      <c r="C38" s="4" t="s">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="6"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="D39" s="4" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="7"/>
-      <c r="B39" s="6"/>
-      <c r="C39" s="1" t="s">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="6"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D40" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A40" s="7">
+    <row r="41" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A41" s="6">
         <v>7</v>
       </c>
-      <c r="B40" s="6" t="s">
+      <c r="B41" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C41" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="D41" s="10" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="7"/>
-      <c r="B41" s="6"/>
-      <c r="C41" s="4" t="s">
+      <c r="E41" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="6"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D41" s="4" t="s">
+      <c r="D42" s="4" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A42" s="7"/>
-      <c r="B42" s="6"/>
-      <c r="C42" s="4" t="s">
+    <row r="43" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A43" s="6"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="D42" s="4" t="s">
+      <c r="D43" s="4" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="7"/>
-      <c r="B43" s="6"/>
-      <c r="C43" s="4" t="s">
+    <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="6"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D43" s="4" t="s">
+      <c r="D44" s="4" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="7"/>
-      <c r="B44" s="6"/>
-      <c r="C44" s="4" t="s">
+    <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="6"/>
+      <c r="B45" s="7"/>
+      <c r="C45" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D44" s="4" t="s">
+      <c r="D45" s="4" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A45" s="7">
+    <row r="46" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A46" s="11">
         <v>8</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="B46" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C46" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D46" s="10" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="7"/>
-      <c r="B46" s="6"/>
-      <c r="C46" s="1" t="s">
+      <c r="E46" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="11"/>
+      <c r="B47" s="12"/>
+      <c r="C47" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="D47" s="10" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A47" s="2">
+      <c r="E47" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A48" s="13">
         <v>9</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B48" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C48" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="D48" s="10" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A48" s="7">
+      <c r="E48" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A49" s="11">
         <v>10</v>
       </c>
-      <c r="B48" s="6" t="s">
+      <c r="B49" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C49" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="D49" s="10" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" s="7"/>
-      <c r="B49" s="6"/>
-      <c r="C49" s="1" t="s">
+      <c r="E49" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" s="11"/>
+      <c r="B50" s="12"/>
+      <c r="C50" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="D50" s="10" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="7"/>
-      <c r="B50" s="6"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="7"/>
-      <c r="B51" s="6"/>
+      <c r="E50" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="11"/>
+      <c r="B51" s="12"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="10"/>
+      <c r="E51" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="11"/>
+      <c r="B52" s="12"/>
+      <c r="C52" s="10"/>
+      <c r="D52" s="10"/>
+      <c r="E52" t="s">
+        <v>110</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A20:A24"/>
-    <mergeCell ref="B20:B24"/>
+    <mergeCell ref="B49:B52"/>
+    <mergeCell ref="A49:A52"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="B41:B45"/>
+    <mergeCell ref="A41:A45"/>
+    <mergeCell ref="B33:B36"/>
+    <mergeCell ref="A33:A36"/>
+    <mergeCell ref="B37:B40"/>
+    <mergeCell ref="A37:A40"/>
+    <mergeCell ref="B26:B32"/>
+    <mergeCell ref="A26:A32"/>
+    <mergeCell ref="A21:A25"/>
+    <mergeCell ref="B21:B25"/>
     <mergeCell ref="B2:B13"/>
     <mergeCell ref="A2:A13"/>
-    <mergeCell ref="B14:B19"/>
-    <mergeCell ref="A14:A19"/>
-    <mergeCell ref="B32:B35"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="B36:B39"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="B25:B31"/>
-    <mergeCell ref="A25:A31"/>
-    <mergeCell ref="B48:B51"/>
-    <mergeCell ref="A48:A51"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B40:B44"/>
-    <mergeCell ref="A40:A44"/>
+    <mergeCell ref="B14:B20"/>
+    <mergeCell ref="A14:A20"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
NC-2.7 - Rotina de validação de email cadastrado
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\AppNotificacoesCrimesCidade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F15F4D40-F897-4647-B623-F1301235B13D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49FF1F19-BFA0-48F6-9199-67E39F813AF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{996D4097-5510-4348-97EC-A204A307EBA8}"/>
   </bookViews>
@@ -448,18 +448,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -470,10 +458,22 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -811,8 +811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94151779-DED3-44C5-B19B-FEA501E890E9}">
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="C19:D19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -838,10 +838,10 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
+      <c r="A2" s="12">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="11" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -852,8 +852,8 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="7"/>
+      <c r="A3" s="12"/>
+      <c r="B3" s="11"/>
       <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
@@ -862,8 +862,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="7"/>
+      <c r="A4" s="12"/>
+      <c r="B4" s="11"/>
       <c r="C4" s="4" t="s">
         <v>5</v>
       </c>
@@ -872,8 +872,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="7"/>
+      <c r="A5" s="12"/>
+      <c r="B5" s="11"/>
       <c r="C5" s="4" t="s">
         <v>6</v>
       </c>
@@ -882,8 +882,8 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="7"/>
+      <c r="A6" s="12"/>
+      <c r="B6" s="11"/>
       <c r="C6" s="4" t="s">
         <v>7</v>
       </c>
@@ -892,8 +892,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="7"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="11"/>
       <c r="C7" s="4" t="s">
         <v>8</v>
       </c>
@@ -902,8 +902,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="7"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="11"/>
       <c r="C8" s="4" t="s">
         <v>9</v>
       </c>
@@ -912,8 +912,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="7"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="11"/>
       <c r="C9" s="4" t="s">
         <v>10</v>
       </c>
@@ -922,8 +922,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="7"/>
+      <c r="A10" s="12"/>
+      <c r="B10" s="11"/>
       <c r="C10" s="4" t="s">
         <v>11</v>
       </c>
@@ -932,8 +932,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="7"/>
+      <c r="A11" s="12"/>
+      <c r="B11" s="11"/>
       <c r="C11" s="4" t="s">
         <v>96</v>
       </c>
@@ -942,8 +942,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="7"/>
+      <c r="A12" s="12"/>
+      <c r="B12" s="11"/>
       <c r="C12" s="4" t="s">
         <v>101</v>
       </c>
@@ -952,8 +952,8 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="7"/>
+      <c r="A13" s="12"/>
+      <c r="B13" s="11"/>
       <c r="C13" s="5" t="s">
         <v>104</v>
       </c>
@@ -962,10 +962,10 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
+      <c r="A14" s="12">
         <v>2</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="11" t="s">
         <v>23</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -976,8 +976,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="7"/>
+      <c r="A15" s="12"/>
+      <c r="B15" s="11"/>
       <c r="C15" s="4" t="s">
         <v>25</v>
       </c>
@@ -986,8 +986,8 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="7"/>
+      <c r="A16" s="12"/>
+      <c r="B16" s="11"/>
       <c r="C16" s="4" t="s">
         <v>26</v>
       </c>
@@ -996,8 +996,8 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="B17" s="7"/>
+      <c r="A17" s="12"/>
+      <c r="B17" s="11"/>
       <c r="C17" s="4" t="s">
         <v>27</v>
       </c>
@@ -1006,12 +1006,12 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="10" t="s">
+      <c r="A18" s="12"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="6" t="s">
         <v>33</v>
       </c>
       <c r="E18" t="s">
@@ -1019,8 +1019,8 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="7"/>
+      <c r="A19" s="12"/>
+      <c r="B19" s="11"/>
       <c r="C19" s="4" t="s">
         <v>106</v>
       </c>
@@ -1029,8 +1029,8 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-      <c r="B20" s="7"/>
+      <c r="A20" s="12"/>
+      <c r="B20" s="11"/>
       <c r="C20" s="1" t="s">
         <v>111</v>
       </c>
@@ -1039,10 +1039,10 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="6">
+      <c r="A21" s="12">
         <v>3</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="11" t="s">
         <v>34</v>
       </c>
       <c r="C21" s="4" t="s">
@@ -1053,8 +1053,8 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="7"/>
+      <c r="A22" s="12"/>
+      <c r="B22" s="11"/>
       <c r="C22" s="4" t="s">
         <v>36</v>
       </c>
@@ -1063,8 +1063,8 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-      <c r="B23" s="7"/>
+      <c r="A23" s="12"/>
+      <c r="B23" s="11"/>
       <c r="C23" s="4" t="s">
         <v>37</v>
       </c>
@@ -1073,8 +1073,8 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="B24" s="7"/>
+      <c r="A24" s="12"/>
+      <c r="B24" s="11"/>
       <c r="C24" s="4" t="s">
         <v>38</v>
       </c>
@@ -1083,8 +1083,8 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
-      <c r="B25" s="7"/>
+      <c r="A25" s="12"/>
+      <c r="B25" s="11"/>
       <c r="C25" s="5" t="s">
         <v>99</v>
       </c>
@@ -1093,10 +1093,10 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="6">
+      <c r="A26" s="12">
         <v>4</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="11" t="s">
         <v>43</v>
       </c>
       <c r="C26" s="4" t="s">
@@ -1107,8 +1107,8 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-      <c r="B27" s="7"/>
+      <c r="A27" s="12"/>
+      <c r="B27" s="11"/>
       <c r="C27" s="4" t="s">
         <v>45</v>
       </c>
@@ -1117,8 +1117,8 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-      <c r="B28" s="7"/>
+      <c r="A28" s="12"/>
+      <c r="B28" s="11"/>
       <c r="C28" s="4" t="s">
         <v>46</v>
       </c>
@@ -1127,8 +1127,8 @@
       </c>
     </row>
     <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
-      <c r="B29" s="7"/>
+      <c r="A29" s="12"/>
+      <c r="B29" s="11"/>
       <c r="C29" s="4" t="s">
         <v>47</v>
       </c>
@@ -1137,8 +1137,8 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="6"/>
-      <c r="B30" s="7"/>
+      <c r="A30" s="12"/>
+      <c r="B30" s="11"/>
       <c r="C30" s="4" t="s">
         <v>48</v>
       </c>
@@ -1147,8 +1147,8 @@
       </c>
     </row>
     <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="6"/>
-      <c r="B31" s="7"/>
+      <c r="A31" s="12"/>
+      <c r="B31" s="11"/>
       <c r="C31" s="4" t="s">
         <v>49</v>
       </c>
@@ -1157,12 +1157,12 @@
       </c>
     </row>
     <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="6"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="10" t="s">
+      <c r="A32" s="12"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="D32" s="10" t="s">
+      <c r="D32" s="6" t="s">
         <v>103</v>
       </c>
       <c r="E32" t="s">
@@ -1170,10 +1170,10 @@
       </c>
     </row>
     <row r="33" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="9">
+      <c r="A33" s="14">
         <v>5</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="13" t="s">
         <v>56</v>
       </c>
       <c r="C33" s="4" t="s">
@@ -1184,8 +1184,8 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="9"/>
-      <c r="B34" s="8"/>
+      <c r="A34" s="14"/>
+      <c r="B34" s="13"/>
       <c r="C34" s="4" t="s">
         <v>58</v>
       </c>
@@ -1194,8 +1194,8 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="9"/>
-      <c r="B35" s="8"/>
+      <c r="A35" s="14"/>
+      <c r="B35" s="13"/>
       <c r="C35" s="4" t="s">
         <v>59</v>
       </c>
@@ -1204,8 +1204,8 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="9"/>
-      <c r="B36" s="8"/>
+      <c r="A36" s="14"/>
+      <c r="B36" s="13"/>
       <c r="C36" s="4" t="s">
         <v>60</v>
       </c>
@@ -1214,10 +1214,10 @@
       </c>
     </row>
     <row r="37" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="6">
+      <c r="A37" s="12">
         <v>6</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="B37" s="11" t="s">
         <v>65</v>
       </c>
       <c r="C37" s="4" t="s">
@@ -1228,8 +1228,8 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="6"/>
-      <c r="B38" s="7"/>
+      <c r="A38" s="12"/>
+      <c r="B38" s="11"/>
       <c r="C38" s="4" t="s">
         <v>67</v>
       </c>
@@ -1238,8 +1238,8 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="6"/>
-      <c r="B39" s="7"/>
+      <c r="A39" s="12"/>
+      <c r="B39" s="11"/>
       <c r="C39" s="4" t="s">
         <v>68</v>
       </c>
@@ -1248,8 +1248,8 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="6"/>
-      <c r="B40" s="7"/>
+      <c r="A40" s="12"/>
+      <c r="B40" s="11"/>
       <c r="C40" s="1" t="s">
         <v>69</v>
       </c>
@@ -1258,16 +1258,16 @@
       </c>
     </row>
     <row r="41" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A41" s="6">
+      <c r="A41" s="12">
         <v>7</v>
       </c>
-      <c r="B41" s="7" t="s">
+      <c r="B41" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="C41" s="10" t="s">
+      <c r="C41" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="D41" s="10" t="s">
+      <c r="D41" s="6" t="s">
         <v>78</v>
       </c>
       <c r="E41" t="s">
@@ -1275,8 +1275,8 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="6"/>
-      <c r="B42" s="7"/>
+      <c r="A42" s="12"/>
+      <c r="B42" s="11"/>
       <c r="C42" s="4" t="s">
         <v>75</v>
       </c>
@@ -1285,8 +1285,8 @@
       </c>
     </row>
     <row r="43" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A43" s="6"/>
-      <c r="B43" s="7"/>
+      <c r="A43" s="12"/>
+      <c r="B43" s="11"/>
       <c r="C43" s="4" t="s">
         <v>77</v>
       </c>
@@ -1295,8 +1295,8 @@
       </c>
     </row>
     <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="6"/>
-      <c r="B44" s="7"/>
+      <c r="A44" s="12"/>
+      <c r="B44" s="11"/>
       <c r="C44" s="4" t="s">
         <v>81</v>
       </c>
@@ -1305,8 +1305,8 @@
       </c>
     </row>
     <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="6"/>
-      <c r="B45" s="7"/>
+      <c r="A45" s="12"/>
+      <c r="B45" s="11"/>
       <c r="C45" s="4" t="s">
         <v>108</v>
       </c>
@@ -1315,16 +1315,16 @@
       </c>
     </row>
     <row r="46" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A46" s="11">
+      <c r="A46" s="10">
         <v>8</v>
       </c>
-      <c r="B46" s="12" t="s">
+      <c r="B46" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="C46" s="10" t="s">
+      <c r="C46" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="D46" s="10" t="s">
+      <c r="D46" s="6" t="s">
         <v>86</v>
       </c>
       <c r="E46" t="s">
@@ -1332,12 +1332,12 @@
       </c>
     </row>
     <row r="47" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A47" s="11"/>
-      <c r="B47" s="12"/>
-      <c r="C47" s="10" t="s">
+      <c r="A47" s="10"/>
+      <c r="B47" s="9"/>
+      <c r="C47" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="D47" s="10" t="s">
+      <c r="D47" s="6" t="s">
         <v>87</v>
       </c>
       <c r="E47" t="s">
@@ -1345,16 +1345,16 @@
       </c>
     </row>
     <row r="48" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A48" s="13">
+      <c r="A48" s="7">
         <v>9</v>
       </c>
-      <c r="B48" s="14" t="s">
+      <c r="B48" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="C48" s="10" t="s">
+      <c r="C48" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="D48" s="10" t="s">
+      <c r="D48" s="6" t="s">
         <v>90</v>
       </c>
       <c r="E48" t="s">
@@ -1362,16 +1362,16 @@
       </c>
     </row>
     <row r="49" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A49" s="11">
+      <c r="A49" s="10">
         <v>10</v>
       </c>
-      <c r="B49" s="12" t="s">
+      <c r="B49" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="C49" s="10" t="s">
+      <c r="C49" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="D49" s="10" t="s">
+      <c r="D49" s="6" t="s">
         <v>94</v>
       </c>
       <c r="E49" t="s">
@@ -1379,12 +1379,12 @@
       </c>
     </row>
     <row r="50" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="11"/>
-      <c r="B50" s="12"/>
-      <c r="C50" s="10" t="s">
+      <c r="A50" s="10"/>
+      <c r="B50" s="9"/>
+      <c r="C50" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="D50" s="10" t="s">
+      <c r="D50" s="6" t="s">
         <v>95</v>
       </c>
       <c r="E50" t="s">
@@ -1392,43 +1392,43 @@
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="11"/>
-      <c r="B51" s="12"/>
-      <c r="C51" s="10"/>
-      <c r="D51" s="10"/>
+      <c r="A51" s="10"/>
+      <c r="B51" s="9"/>
+      <c r="C51" s="6"/>
+      <c r="D51" s="6"/>
       <c r="E51" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="11"/>
-      <c r="B52" s="12"/>
-      <c r="C52" s="10"/>
-      <c r="D52" s="10"/>
+      <c r="A52" s="10"/>
+      <c r="B52" s="9"/>
+      <c r="C52" s="6"/>
+      <c r="D52" s="6"/>
       <c r="E52" t="s">
         <v>110</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A21:A25"/>
+    <mergeCell ref="B21:B25"/>
+    <mergeCell ref="B2:B13"/>
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="B14:B20"/>
+    <mergeCell ref="A14:A20"/>
+    <mergeCell ref="B33:B36"/>
+    <mergeCell ref="A33:A36"/>
+    <mergeCell ref="B37:B40"/>
+    <mergeCell ref="A37:A40"/>
+    <mergeCell ref="B26:B32"/>
+    <mergeCell ref="A26:A32"/>
     <mergeCell ref="B49:B52"/>
     <mergeCell ref="A49:A52"/>
     <mergeCell ref="B46:B47"/>
     <mergeCell ref="A46:A47"/>
     <mergeCell ref="B41:B45"/>
     <mergeCell ref="A41:A45"/>
-    <mergeCell ref="B33:B36"/>
-    <mergeCell ref="A33:A36"/>
-    <mergeCell ref="B37:B40"/>
-    <mergeCell ref="A37:A40"/>
-    <mergeCell ref="B26:B32"/>
-    <mergeCell ref="A26:A32"/>
-    <mergeCell ref="A21:A25"/>
-    <mergeCell ref="B21:B25"/>
-    <mergeCell ref="B2:B13"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="B14:B20"/>
-    <mergeCell ref="A14:A20"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
NC-3.5 - Ajustado credenciais da aplicação para váriaveis de ambiente
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\AppNotificacoesCrimesCidade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49FF1F19-BFA0-48F6-9199-67E39F813AF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F40AFE9-CBFE-4D29-8CB8-99FD32D3A217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{996D4097-5510-4348-97EC-A204A307EBA8}"/>
+    <workbookView xWindow="-21720" yWindow="-1545" windowWidth="21840" windowHeight="13140" xr2:uid="{996D4097-5510-4348-97EC-A204A307EBA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -811,8 +811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94151779-DED3-44C5-B19B-FEA501E890E9}">
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="D25" sqref="C25:D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1031,10 +1031,10 @@
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="12"/>
       <c r="B20" s="11"/>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="4" t="s">
         <v>112</v>
       </c>
     </row>
@@ -1085,10 +1085,10 @@
     <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="12"/>
       <c r="B25" s="11"/>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="4" t="s">
         <v>98</v>
       </c>
     </row>

</xml_diff>